<commit_message>
updated jaw dimensions and dial limits
</commit_message>
<xml_diff>
--- a/EEmapping.xlsx
+++ b/EEmapping.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/arion_law_mail_utoronto_ca/Documents/SickKids/Continuum_Tool_Modeling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arion Law\OneDrive - University of Toronto\SickKids\Continuum_Tool_Modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F6F97407-A413-4288-8572-14C58B4E9A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24398" yWindow="-98" windowWidth="24496" windowHeight="15675"/>
+    <workbookView xWindow="-24405" yWindow="-105" windowWidth="24495" windowHeight="15675"/>
   </bookViews>
   <sheets>
     <sheet name="EEmapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -585,6 +584,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2982,6 +2982,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2989,7 +2990,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3918,15 +3918,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C362"/>
+  <dimension ref="A1:E362"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F178" sqref="F178"/>
+      <selection activeCell="E284" sqref="E284"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>-2.597118408</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>-2.5958444049999998</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>-2.5945118489999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>-2.5931157800000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>-2.5916513170000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>-2.5901136550000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>-2.5884980660000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>-2.586799901</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>-2.5850145879999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>-2.5831376330000002</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>-2.58116462</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>-2.5790912110000002</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>-2.5769131449999998</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>-2.5746262400000002</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>-2.5722263910000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>-2.5697095669999999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>-2.5670718190000001</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>-2.5643092689999998</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>-2.5614181180000002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>-2.5583946420000001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>-2.5552351889999998</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>-2.5519361859999998</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>-2.5484941299999999</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>-2.5449055920000001</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>-2.5411672150000002</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>-2.5372757159999999</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>-2.5332278800000001</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>-2.5290205650000002</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>-2.5246506970000002</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>-2.5201152709999999</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>-2.5154113520000001</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>-2.5105360710000002</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>-2.5054866260000002</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>-2.5002602820000002</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>-2.4948543669999999</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>-2.4892662759999999</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>-2.4834934670000002</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>-2.477533459</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>-2.4713838359999998</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>-2.465042242</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>-2.4585063819999999</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>-2.4517740200000002</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>-2.4448429800000002</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>-2.4377111440000001</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>-2.430376452</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>-2.4228369010000002</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>-2.4150905429999998</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>-2.4071354870000001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>-2.3989698939999999</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>-2.3905919820000001</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>-2.3820000210000001</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>-2.3731923319999999</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>-2.3641672890000001</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>-2.3549233190000001</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>-2.3454588959999998</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>-2.3357725459999998</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>-2.325862844</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>-2.3157284119999999</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>-2.3053679210000002</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>-2.2947800900000002</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>-2.283963682</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>-2.2729175079999999</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>-2.261640425</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>-2.250131332</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>-2.238389175</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>-2.2264129420000001</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>-2.214201664</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>-2.201754416</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>-2.1890703130000002</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>-2.1761485139999999</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>-2.162988216</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>-2.1495886579999999</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>-2.1359491199999998</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>-2.1220689190000002</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>-2.1079474130000002</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>-2.0935839970000001</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>-2.078978105</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>-2.0641292099999999</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>-2.0490368179999998</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>-2.033700477</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>-2.018119767</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>-2.002294306</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>-1.9862237460000001</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>-1.9699077780000001</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>-1.953346123</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>-1.936538538</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>-1.919484816</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>-1.9021847810000001</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>-1.8846382909999999</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>-1.866845238</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>-1.8488055450000001</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>-1.8305191700000001</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>-1.8119860990000001</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>-1.793206353</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>-1.774179983</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>-1.7549070710000001</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>-1.7353877310000001</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>-1.715622105</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>-1.6956103680000001</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>-1.675352723</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>-1.6548494039999999</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>-1.6341006730000001</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>-1.6131068230000001</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>-1.591868174</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>-1.570385076</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>-1.5486579069999999</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>-1.526687074</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>-1.5044730100000001</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>-1.4820161780000001</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>-1.4593170680000001</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>-1.436376197</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
@@ -5166,7 +5166,7 @@
         <v>-1.413194109</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>-1.3897713759999999</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>-1.366108595</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>-1.3422063909999999</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>-1.318065416</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>-1.2936863460000001</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>-1.269069885</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>-1.2442167630000001</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>-1.219127734</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>-1.19380358</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>121</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>-1.168245105</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>122</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>-1.1424531419999999</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>123</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>-1.116428548</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>124</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>-1.090172202</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>125</v>
       </c>
@@ -5320,7 +5320,7 @@
         <v>-1.0636850120000001</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>126</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>-1.036967908</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>-1.0100218459999999</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>128</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>-0.98284780599999999</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>129</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>-0.95544679099999996</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>130</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>-0.92781983000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>131</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>-0.89996797500000003</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>132</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>-0.87189230200000001</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>133</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>-0.84359390999999995</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>134</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>-0.81507392400000001</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>135</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>-0.786333489</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>136</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>-0.75737377699999997</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>137</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>-0.72819598200000002</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>138</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>-0.698801318</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>139</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>-0.66919102799999997</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>140</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>-0.63936637299999999</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>141</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>-0.60932863900000001</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>142</v>
       </c>
@@ -5507,7 +5507,7 @@
         <v>-0.579079134</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>143</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>-0.54861918899999995</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>144</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>-0.51795015799999999</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>145</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>-0.48707341599999998</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>146</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>-0.45599036199999998</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>147</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>-0.424702415</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>148</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>-0.39321102000000002</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>149</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>-0.361517639</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>150</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>-0.32962375900000002</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>151</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>-0.29753088900000002</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>152</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>-0.26524055899999999</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>153</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>-0.23275431899999999</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>154</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>-0.200073742</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>155</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>-0.16720042500000001</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>156</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>-0.13413598099999999</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>157</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>-0.100882048</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>158</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>-6.7440284000000003E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>159</v>
       </c>
@@ -5694,7 +5694,7 @@
         <v>-3.3812368000000002E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>160</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>3.9699999999999997E-14</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>161</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>3.3995099000000001E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>162</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>6.8171186999999994E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>163</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>0.102526503</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>164</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>0.13705926299999999</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>165</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>0.17176766500000001</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>166</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>0.20664988500000001</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>167</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>0.24170407899999999</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>168</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>0.276928383</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>169</v>
       </c>
@@ -5804,7 +5804,7 @@
         <v>0.31232091400000001</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>170</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>0.34787976700000001</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>171</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>0.38360302000000002</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>172</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>0.41948872799999998</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>173</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>0.45553492899999998</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>174</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>0.49173964100000001</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>175</v>
       </c>
@@ -5870,7 +5870,7 @@
         <v>0.52810086099999998</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>176</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>0.56461656900000001</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>177</v>
       </c>
@@ -5892,7 +5892,7 @@
         <v>0.60128472399999999</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>178</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>0.63810326799999995</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>179</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>0.67507012099999997</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>180</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>0.71218318700000005</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>181</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>0.74944034999999998</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>182</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>0.78683947499999995</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>183</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>0.82437841099999998</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>184</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>0.86205498599999997</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>185</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>0.89986701099999999</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>186</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>0.937812278</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>187</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>0.97588856199999996</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>188</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>1.0140936199999999</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>189</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>1.052425191</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>190</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>1.090880997</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>191</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>1.129458742</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>192</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>1.168156113</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>193</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>1.20697078</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>194</v>
       </c>
@@ -6079,7 +6079,7 @@
         <v>1.2459003959999999</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>195</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>1.2849425969999999</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>196</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>1.324095002</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>197</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>1.3633552149999999</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>198</v>
       </c>
@@ -6123,7 +6123,7 @@
         <v>1.402720822</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>199</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>1.442189393</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>200</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>1.481758482</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>201</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>1.521425628</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>202</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>1.561188354</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>203</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>1.6010441660000001</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>204</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>1.6409905570000001</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>205</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>1.6810250019999999</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>206</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>1.7211449640000001</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>207</v>
       </c>
@@ -6222,7 +6222,7 @@
         <v>1.7613478899999999</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>208</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>1.80163121</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>209</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>1.841992343</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>210</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>1.882428692</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>211</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>1.9229376469999999</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>212</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>1.9635165809999999</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>213</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>2.0041628579999999</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>214</v>
       </c>
@@ -6299,7 +6299,7 @@
         <v>2.0448738240000002</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>215</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>2.0856468160000001</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>216</v>
       </c>
@@ -6321,7 +6321,7 @@
         <v>2.126479153</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>217</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>2.1673681459999998</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>218</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>2.20831109</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>219</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>2.2493052680000001</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>220</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>2.2903479529999999</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>221</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>2.3314364040000002</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>222</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>2.3725678669999999</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>223</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>2.4137395800000001</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>224</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>2.4549487669999999</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>225</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>2.4961926409999999</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>226</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>2.5374684049999998</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>227</v>
       </c>
@@ -6442,7 +6442,7 @@
         <v>2.578773252</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>228</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>2.6201043620000002</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>229</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>2.6614589080000002</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>230</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>2.702834051</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>231</v>
       </c>
@@ -6486,7 +6486,7 @@
         <v>2.7442269439999998</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>232</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>2.7856347279999998</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>233</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>2.827054537</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>234</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>2.8684834970000002</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>235</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>2.9099187230000001</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>236</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>2.9513573219999998</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>237</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>2.9927963960000001</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>238</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>3.0342330340000001</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>239</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>3.0756643229999998</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>240</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>3.1170873380000002</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>241</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>3.1584991499999999</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>242</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>3.199896823</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>243</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>3.2412774139999998</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>244</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>3.2826379729999999</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>245</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>3.3239755459999998</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>246</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>3.3652871719999999</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>247</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>3.4065698869999999</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>248</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>3.447820718</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>249</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>3.489036692</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>250</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>3.5302148290000002</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>251</v>
       </c>
@@ -6706,7 +6706,7 @@
         <v>3.5713521450000001</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>252</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>3.6124456540000001</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>253</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>3.6534923639999999</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>254</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>3.6944892820000002</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>255</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>3.7354334119999999</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>256</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>3.7763217550000001</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>257</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>3.8171513090000002</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>258</v>
       </c>
@@ -6783,7 +6783,7 @@
         <v>3.8579190730000001</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>259</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>3.8986220409999999</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>260</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>3.939257209</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>261</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>3.9798215689999998</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>262</v>
       </c>
@@ -6827,7 +6827,7 @@
         <v>4.0203121160000004</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>263</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>4.0607258420000001</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>264</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>4.1010597410000003</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>265</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>4.1413108059999999</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>266</v>
       </c>
@@ -6871,7 +6871,7 @@
         <v>4.1814760309999999</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>267</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>4.2215524120000003</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>268</v>
       </c>
@@ -6893,7 +6893,7 @@
         <v>4.2615369469999997</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>269</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>4.3014266340000002</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>270</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>4.3412184739999997</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>271</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>4.3809094719999999</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>272</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>4.420496633</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>273</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>4.4599769670000002</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>274</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>4.4993474879999997</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>275</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>4.5386052120000002</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>276</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>4.5777471609999996</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>277</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>4.6167703610000004</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>278</v>
       </c>
@@ -7003,7 +7003,7 @@
         <v>4.6556718430000004</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>279</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>4.6944486430000003</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>280</v>
       </c>
@@ -7025,7 +7025,7 @@
         <v>4.7330978029999997</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>281</v>
       </c>
@@ -7036,7 +7036,7 @@
         <v>4.7716163690000002</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>282</v>
       </c>
@@ -7046,8 +7046,12 @@
       <c r="C284">
         <v>4.7907056639999999</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E284">
+        <f>DEGREES(B284)</f>
+        <v>51.000000027667674</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>283</v>
       </c>
@@ -7058,7 +7062,7 @@
         <v>4.7870027349999997</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>284</v>
       </c>
@@ -7069,7 +7073,7 @@
         <v>4.7831571190000002</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>285</v>
       </c>
@@ -7080,7 +7084,7 @@
         <v>4.7791689689999997</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>286</v>
       </c>
@@ -7091,7 +7095,7 @@
         <v>4.7750384549999998</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>287</v>
       </c>
@@ -7102,7 +7106,7 @@
         <v>4.7707657640000001</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>288</v>
       </c>
@@ -7113,7 +7117,7 @@
         <v>4.7663510980000003</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>289</v>
       </c>
@@ -7124,7 +7128,7 @@
         <v>4.7617946739999999</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>290</v>
       </c>
@@ -7135,7 +7139,7 @@
         <v>4.7570967279999996</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>291</v>
       </c>
@@ -7146,7 +7150,7 @@
         <v>4.7522575089999997</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>292</v>
       </c>
@@ -7157,7 +7161,7 @@
         <v>4.7472772829999998</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>293</v>
       </c>
@@ -7168,7 +7172,7 @@
         <v>4.7421563310000003</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>294</v>
       </c>
@@ -7179,7 +7183,7 @@
         <v>4.7368949530000002</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>295</v>
       </c>
@@ -7190,7 +7194,7 @@
         <v>4.7314934620000004</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>296</v>
       </c>
@@ -7201,7 +7205,7 @@
         <v>4.725952189</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>297</v>
       </c>
@@ -7212,7 +7216,7 @@
         <v>4.720271479</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>298</v>
       </c>
@@ -7223,7 +7227,7 @@
         <v>4.7144516950000002</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>299</v>
       </c>
@@ -7234,7 +7238,7 @@
         <v>4.7084932149999998</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>300</v>
       </c>
@@ -7245,7 +7249,7 @@
         <v>4.7023964349999998</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>301</v>
       </c>
@@ -7256,7 +7260,7 @@
         <v>4.6961617640000002</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>302</v>
       </c>
@@ -7267,7 +7271,7 @@
         <v>4.6897896299999999</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>303</v>
       </c>
@@ -7278,7 +7282,7 @@
         <v>4.6832804760000002</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>304</v>
       </c>
@@ -7289,7 +7293,7 @@
         <v>4.6766347609999999</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>305</v>
       </c>
@@ -7300,7 +7304,7 @@
         <v>4.6698529610000001</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>306</v>
       </c>
@@ -7311,7 +7315,7 @@
         <v>4.6629355669999999</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>307</v>
       </c>
@@ -7322,7 +7326,7 @@
         <v>4.6558830889999996</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>308</v>
       </c>
@@ -7333,7 +7337,7 @@
         <v>4.6486960499999999</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>309</v>
       </c>
@@ -7344,7 +7348,7 @@
         <v>4.6413749920000003</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>310</v>
       </c>
@@ -7355,7 +7359,7 @@
         <v>4.6339204709999997</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>311</v>
       </c>
@@ -7366,7 +7370,7 @@
         <v>4.6263330610000004</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>312</v>
       </c>
@@ -7377,7 +7381,7 @@
         <v>4.6186133529999998</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>313</v>
       </c>
@@ -7388,7 +7392,7 @@
         <v>4.6107619529999999</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>314</v>
       </c>
@@ -7399,7 +7403,7 @@
         <v>4.602779484</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>315</v>
       </c>
@@ -7410,7 +7414,7 @@
         <v>4.5946665859999998</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>316</v>
       </c>
@@ -7421,7 +7425,7 @@
         <v>4.5864239160000002</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>317</v>
       </c>
@@ -7432,7 +7436,7 @@
         <v>4.578052145</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>318</v>
       </c>
@@ -7443,7 +7447,7 @@
         <v>4.5695519640000004</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>319</v>
       </c>
@@ -7454,7 +7458,7 @@
         <v>4.5609240790000003</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>320</v>
       </c>
@@ -7465,7 +7469,7 @@
         <v>4.5521692119999999</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>321</v>
       </c>
@@ -7476,7 +7480,7 @@
         <v>4.5432881040000002</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>322</v>
       </c>
@@ -7487,7 +7491,7 @@
         <v>4.5342815109999997</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>323</v>
       </c>
@@ -7498,7 +7502,7 @@
         <v>4.5251502060000002</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>324</v>
       </c>
@@ -7509,7 +7513,7 @@
         <v>4.5158949799999997</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>325</v>
       </c>
@@ -7520,7 +7524,7 @@
         <v>4.5065166400000001</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>326</v>
       </c>
@@ -7531,7 +7535,7 @@
         <v>4.4970160110000004</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>327</v>
       </c>
@@ -7542,7 +7546,7 @@
         <v>4.4873939319999998</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>328</v>
       </c>
@@ -7553,7 +7557,7 @@
         <v>4.4776512640000004</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>329</v>
       </c>
@@ -7564,7 +7568,7 @@
         <v>4.4677888799999996</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>330</v>
       </c>
@@ -7575,7 +7579,7 @@
         <v>4.4578076749999997</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>331</v>
       </c>
@@ -7586,7 +7590,7 @@
         <v>4.4477085580000004</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>332</v>
       </c>
@@ -7597,7 +7601,7 @@
         <v>4.4374924560000002</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>333</v>
       </c>
@@ -7608,7 +7612,7 @@
         <v>4.4271603129999999</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>334</v>
       </c>
@@ -7619,7 +7623,7 @@
         <v>4.4167130920000002</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>335</v>
       </c>
@@ -7630,7 +7634,7 @@
         <v>4.4061517720000003</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>336</v>
       </c>
@@ -7641,7 +7645,7 @@
         <v>4.3954773490000001</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>337</v>
       </c>
@@ -7652,7 +7656,7 @@
         <v>4.3846908400000002</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>338</v>
       </c>
@@ -7663,7 +7667,7 @@
         <v>4.3737932739999996</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>339</v>
       </c>
@@ -7674,7 +7678,7 @@
         <v>4.3627857030000001</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>340</v>
       </c>
@@ -7685,7 +7689,7 @@
         <v>4.3516691940000003</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>341</v>
       </c>
@@ -7696,7 +7700,7 @@
         <v>4.3404448320000002</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>342</v>
       </c>
@@ -7707,7 +7711,7 @@
         <v>4.3291137209999997</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>343</v>
       </c>
@@ -7718,7 +7722,7 @@
         <v>4.317676981</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>344</v>
       </c>
@@ -7729,7 +7733,7 @@
         <v>4.3061357530000004</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>345</v>
       </c>
@@ -7740,7 +7744,7 @@
         <v>4.2944911929999998</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>346</v>
       </c>
@@ -7751,7 +7755,7 @@
         <v>4.2827444769999996</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>347</v>
       </c>
@@ -7762,7 +7766,7 @@
         <v>4.270896799</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>348</v>
       </c>
@@ -7773,7 +7777,7 @@
         <v>4.2589493709999999</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>349</v>
       </c>
@@ -7784,7 +7788,7 @@
         <v>4.246903423</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>350</v>
       </c>
@@ -7795,7 +7799,7 @@
         <v>4.2347602039999996</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>351</v>
       </c>
@@ -7806,7 +7810,7 @@
         <v>4.2225209819999998</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>352</v>
       </c>
@@ -7817,7 +7821,7 @@
         <v>4.2101870420000003</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>353</v>
       </c>
@@ -7828,7 +7832,7 @@
         <v>4.1977596899999998</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>354</v>
       </c>
@@ -7839,7 +7843,7 @@
         <v>4.1852402489999996</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>355</v>
       </c>
@@ -7850,7 +7854,7 @@
         <v>4.1726300609999996</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>356</v>
       </c>
@@ -7861,7 +7865,7 @@
         <v>4.1599304879999996</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>357</v>
       </c>
@@ -7872,7 +7876,7 @@
         <v>4.1471429100000003</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>358</v>
       </c>
@@ -7883,7 +7887,7 @@
         <v>4.1342687260000002</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>359</v>
       </c>
@@ -7894,7 +7898,7 @@
         <v>4.1213093550000002</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>360</v>
       </c>

</xml_diff>

<commit_message>
fixed linear interpolation to work for both increasing and decreasing functions || fixed jaw angle FK for angles < 0deg
</commit_message>
<xml_diff>
--- a/EEmapping.xlsx
+++ b/EEmapping.xlsx
@@ -1,20 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arion Law\OneDrive - University of Toronto\SickKids\Continuum_Tool_Modeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/arion_law_mail_utoronto_ca/Documents/SickKids/Continuum_Tool_Modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_FBD155BEA7D03DDB4F840A77004E59CE1208E59B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F73D257-2855-4A09-8792-FFB9A9174983}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EEmapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -57,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -10575,7 +10589,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10693,7 +10706,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10815,7 +10827,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -10823,6 +10834,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -11418,15 +11430,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>45983</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>3260</xdr:rowOff>
+      <xdr:colOff>289244</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76147</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>350784</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>252786</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>72886</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11750,11 +11762,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J542"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
implemented linear approximation for cable length to wrist pseudjoint angle allocation
</commit_message>
<xml_diff>
--- a/EEmapping.xlsx
+++ b/EEmapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/arion_law_mail_utoronto_ca/Documents/SickKids/Continuum_Tool_Modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_FBD155BEA7D03DDB4F840A77004E59CE1208E59B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F73D257-2855-4A09-8792-FFB9A9174983}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_FBD155BEA7D03DDB4F840A77004E59CE1208E59B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4051E970-1047-480B-A19A-85C6C246ECE3}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-20412" yWindow="0" windowWidth="21600" windowHeight="9996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EEmapping" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Disk2Angle</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Quadratic</t>
+  </si>
+  <si>
+    <t>setpoint</t>
   </si>
 </sst>
 </file>
@@ -11763,10 +11766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J542"/>
+  <dimension ref="A1:N542"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11775,7 +11778,7 @@
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -11795,7 +11798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -11806,11 +11809,11 @@
         <v>2.2341553417272602</v>
       </c>
       <c r="D2">
-        <f>IF(B2&gt;$J$7,$I$2*SIN($I$3*B2+$I$5)+$I$4,$I$9*SIN($I$10*B2+$I$12)+$I$11)</f>
+        <f>IF(B2&gt;($J$7+$M$2),$I$2*SIN($I$3*B2+($I$5-$M$2))+$I$4,$I$9*SIN($I$10*B2+($I$12-$M$2))+$I$11)</f>
         <v>2.2850969501953067</v>
       </c>
       <c r="E2">
-        <f>IF(B2&gt;$J$7,$J$2*(B2+$J$5)^4+$J$4,$J$9*(B2+$J$12)^2+$J$11)</f>
+        <f>IF(B2&gt;($J$7+$M$2),$J$2*(B2+($J$5-$M$2))^2+$J$4,$J$9*(B2+($J$12-$M$2))^2+$J$11)</f>
         <v>2.2793390097549033</v>
       </c>
       <c r="G2" t="s">
@@ -11822,8 +11825,18 @@
       <c r="J2">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <f>RADIANS(N2)</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -11834,11 +11847,11 @@
         <v>2.2434381316832099</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D66" si="0">IF(B3&gt;$J$7,$I$2*SIN($I$3*B3+$I$5)+$I$4,$I$9*SIN($I$10*B3+$I$12)+$I$11)</f>
+        <f t="shared" ref="D3:D66" si="0">IF(B3&gt;($J$7+$M$2),$I$2*SIN($I$3*B3+($I$5-$M$2))+$I$4,$I$9*SIN($I$10*B3+($I$12-$M$2))+$I$11)</f>
         <v>2.2948383110900616</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="1">IF(B3&gt;$J$7,$J$2*(B3+$J$5)^2+$J$4,$J$9*(B3+$J$12)^2+$J$11)</f>
+        <f t="shared" ref="E3:E66" si="1">IF(B3&gt;($J$7+$M$2),$J$2*(B3+($J$5-$M$2))^2+$J$4,$J$9*(B3+($J$12-$M$2))^2+$J$11)</f>
         <v>2.2957578886814036</v>
       </c>
       <c r="G3" t="s">
@@ -11848,7 +11861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -11876,7 +11889,7 @@
         <v>-3.4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -11904,7 +11917,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -11923,7 +11936,7 @@
         <v>2.3446489845571796</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -11952,7 +11965,7 @@
         <v>-0.89011791851710809</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -11971,7 +11984,7 @@
         <v>2.3769384310545645</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -11999,7 +12012,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -12024,7 +12037,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -12052,7 +12065,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -12077,7 +12090,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -12096,7 +12109,7 @@
         <v>2.4565958863287927</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -12115,7 +12128,7 @@
         <v>2.4723446069317618</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -12134,7 +12147,7 @@
         <v>2.4880324040507746</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -13114,11 +13127,11 @@
         <v>3.0713033804556602</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D130" si="2">IF(B67&gt;$J$7,$I$2*SIN($I$3*B67+$I$5)+$I$4,$I$9*SIN($I$10*B67+$I$12)+$I$11)</f>
+        <f t="shared" ref="D67:D130" si="2">IF(B67&gt;($J$7+$M$2),$I$2*SIN($I$3*B67+($I$5-$M$2))+$I$4,$I$9*SIN($I$10*B67+($I$12-$M$2))+$I$11)</f>
         <v>3.1182110705644814</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E130" si="3">IF(B67&gt;$J$7,$J$2*(B67+$J$5)^2+$J$4,$J$9*(B67+$J$12)^2+$J$11)</f>
+        <f t="shared" ref="E67:E130" si="3">IF(B67&gt;($J$7+$M$2),$J$2*(B67+($J$5-$M$2))^2+$J$4,$J$9*(B67+($J$12-$M$2))^2+$J$11)</f>
         <v>3.2198452933463537</v>
       </c>
     </row>
@@ -14330,11 +14343,11 @@
         <v>3.8445850855645798</v>
       </c>
       <c r="D131">
-        <f t="shared" ref="D131:D194" si="4">IF(B131&gt;$J$7,$I$2*SIN($I$3*B131+$I$5)+$I$4,$I$9*SIN($I$10*B131+$I$12)+$I$11)</f>
+        <f t="shared" ref="D131:D194" si="4">IF(B131&gt;($J$7+$M$2),$I$2*SIN($I$3*B131+($I$5-$M$2))+$I$4,$I$9*SIN($I$10*B131+($I$12-$M$2))+$I$11)</f>
         <v>3.9295328582884492</v>
       </c>
       <c r="E131">
-        <f t="shared" ref="E131:E194" si="5">IF(B131&gt;$J$7,$J$2*(B131+$J$5)^2+$J$4,$J$9*(B131+$J$12)^2+$J$11)</f>
+        <f t="shared" ref="E131:E194" si="5">IF(B131&gt;($J$7+$M$2),$J$2*(B131+($J$5-$M$2))^2+$J$4,$J$9*(B131+($J$12-$M$2))^2+$J$11)</f>
         <v>3.8943901077220371</v>
       </c>
     </row>
@@ -15546,11 +15559,11 @@
         <v>3.1167564902052902</v>
       </c>
       <c r="D195">
-        <f t="shared" ref="D195:D258" si="6">IF(B195&gt;$J$7,$I$2*SIN($I$3*B195+$I$5)+$I$4,$I$9*SIN($I$10*B195+$I$12)+$I$11)</f>
+        <f t="shared" ref="D195:D258" si="6">IF(B195&gt;($J$7+$M$2),$I$2*SIN($I$3*B195+($I$5-$M$2))+$I$4,$I$9*SIN($I$10*B195+($I$12-$M$2))+$I$11)</f>
         <v>3.3068282600845826</v>
       </c>
       <c r="E195">
-        <f t="shared" ref="E195:E258" si="7">IF(B195&gt;$J$7,$J$2*(B195+$J$5)^2+$J$4,$J$9*(B195+$J$12)^2+$J$11)</f>
+        <f t="shared" ref="E195:E258" si="7">IF(B195&gt;($J$7+$M$2),$J$2*(B195+($J$5-$M$2))^2+$J$4,$J$9*(B195+($J$12-$M$2))^2+$J$11)</f>
         <v>2.9212817717533635</v>
       </c>
     </row>
@@ -16762,11 +16775,11 @@
         <v>0.49560633956921002</v>
       </c>
       <c r="D259">
-        <f t="shared" ref="D259:D322" si="8">IF(B259&gt;$J$7,$I$2*SIN($I$3*B259+$I$5)+$I$4,$I$9*SIN($I$10*B259+$I$12)+$I$11)</f>
+        <f t="shared" ref="D259:D322" si="8">IF(B259&gt;($J$7+$M$2),$I$2*SIN($I$3*B259+($I$5-$M$2))+$I$4,$I$9*SIN($I$10*B259+($I$12-$M$2))+$I$11)</f>
         <v>0.67010454386605522</v>
       </c>
       <c r="E259">
-        <f t="shared" ref="E259:E322" si="9">IF(B259&gt;$J$7,$J$2*(B259+$J$5)^2+$J$4,$J$9*(B259+$J$12)^2+$J$11)</f>
+        <f t="shared" ref="E259:E322" si="9">IF(B259&gt;($J$7+$M$2),$J$2*(B259+($J$5-$M$2))^2+$J$4,$J$9*(B259+($J$12-$M$2))^2+$J$11)</f>
         <v>8.8300448767401729E-2</v>
       </c>
     </row>
@@ -17978,11 +17991,11 @@
         <v>-1.6637838109206899</v>
       </c>
       <c r="D323">
-        <f t="shared" ref="D323:D386" si="10">IF(B323&gt;$J$7,$I$2*SIN($I$3*B323+$I$5)+$I$4,$I$9*SIN($I$10*B323+$I$12)+$I$11)</f>
+        <f t="shared" ref="D323:D386" si="10">IF(B323&gt;($J$7+$M$2),$I$2*SIN($I$3*B323+($I$5-$M$2))+$I$4,$I$9*SIN($I$10*B323+($I$12-$M$2))+$I$11)</f>
         <v>-1.6840204024823837</v>
       </c>
       <c r="E323">
-        <f t="shared" ref="E323:E361" si="11">IF(B323&gt;$J$7,$J$2*(B323+$J$5)^2+$J$4,$J$9*(B323+$J$12)^2+$J$11)</f>
+        <f t="shared" ref="E323:E386" si="11">IF(B323&gt;($J$7+$M$2),$J$2*(B323+($J$5-$M$2))^2+$J$4,$J$9*(B323+($J$12-$M$2))^2+$J$11)</f>
         <v>-1.9087131967494961</v>
       </c>
     </row>
@@ -18723,7 +18736,7 @@
         <v>-2.6642263173701051</v>
       </c>
       <c r="E362">
-        <f>IF(B362&gt;$J$7,$J$2*(B362+$J$5)^2+$J$4,$J$9*(B362+$J$12)^2+$J$11)</f>
+        <f t="shared" si="11"/>
         <v>-2.7157212482664828</v>
       </c>
     </row>
@@ -18742,7 +18755,7 @@
         <v>-2.6832947738172606</v>
       </c>
       <c r="E363">
-        <f t="shared" ref="E363:E426" si="12">IF(B363&gt;$J$7,$J$2*(B363+$J$5)^2+$J$4,$J$9*(B363+$J$12)^2+$J$11)</f>
+        <f t="shared" si="11"/>
         <v>-2.7323318889828005</v>
       </c>
     </row>
@@ -18761,7 +18774,7 @@
         <v>-2.7020370407839409</v>
       </c>
       <c r="E364">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.7487384360278639</v>
       </c>
     </row>
@@ -18780,7 +18793,7 @@
         <v>-2.720451690973952</v>
       </c>
       <c r="E365">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.7649408894016694</v>
       </c>
     </row>
@@ -18799,7 +18812,7 @@
         <v>-2.738537322040385</v>
       </c>
       <c r="E366">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.7809392491042164</v>
       </c>
     </row>
@@ -18818,7 +18831,7 @@
         <v>-2.7562925566924155</v>
       </c>
       <c r="E367">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.7967335151355077</v>
       </c>
     </row>
@@ -18837,7 +18850,7 @@
         <v>-2.7737160428001819</v>
       </c>
       <c r="E368">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.8123236874955424</v>
       </c>
     </row>
@@ -18856,7 +18869,7 @@
         <v>-2.790806453497757</v>
       </c>
       <c r="E369">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.8277097661843178</v>
       </c>
     </row>
@@ -18875,7 +18888,7 @@
         <v>-2.8075624872842018</v>
       </c>
       <c r="E370">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.8428917512018379</v>
       </c>
     </row>
@@ -18894,7 +18907,7 @@
         <v>-2.8239828681226675</v>
       </c>
       <c r="E371">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.8578696425481009</v>
       </c>
     </row>
@@ -18913,7 +18926,7 @@
         <v>-2.8400663455375788</v>
       </c>
       <c r="E372">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.8726434402231051</v>
       </c>
     </row>
@@ -18932,7 +18945,7 @@
         <v>-2.8558116947098617</v>
       </c>
       <c r="E373">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.8872131442268545</v>
       </c>
     </row>
@@ -18951,7 +18964,7 @@
         <v>-2.8712177165702166</v>
       </c>
       <c r="E374">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.9015787545593459</v>
       </c>
     </row>
@@ -18970,7 +18983,7 @@
         <v>-2.8862832378904293</v>
       </c>
       <c r="E375">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.9157402712205789</v>
       </c>
     </row>
@@ -18989,7 +19002,7 @@
         <v>-2.9010071113727283</v>
       </c>
       <c r="E376">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.9296976942105566</v>
       </c>
     </row>
@@ -19008,7 +19021,7 @@
         <v>-2.9153882157371362</v>
       </c>
       <c r="E377">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.9434510235292772</v>
       </c>
     </row>
@@ -19027,7 +19040,7 @@
         <v>-2.9294254558068791</v>
       </c>
       <c r="E378">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.957000259176739</v>
       </c>
     </row>
@@ -19046,7 +19059,7 @@
         <v>-2.9431177625917804</v>
       </c>
       <c r="E379">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.9703454011529451</v>
       </c>
     </row>
@@ -19065,7 +19078,7 @@
         <v>-2.9564640933696649</v>
       </c>
       <c r="E380">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.9834864494578945</v>
       </c>
     </row>
@@ -19084,7 +19097,7 @@
         <v>-2.9694634317657695</v>
       </c>
       <c r="E381">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2.9964234040915851</v>
       </c>
     </row>
@@ -19103,7 +19116,7 @@
         <v>-2.9821147878301493</v>
       </c>
       <c r="E382">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-3.00915626505402</v>
       </c>
     </row>
@@ -19122,7 +19135,7 @@
         <v>-2.9944171981130565</v>
       </c>
       <c r="E383">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-3.0216850323451965</v>
       </c>
     </row>
@@ -19141,7 +19154,7 @@
         <v>-3.0063697257383191</v>
       </c>
       <c r="E384">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-3.0340097059651172</v>
       </c>
     </row>
@@ -19160,7 +19173,7 @@
         <v>-3.0179714604746803</v>
       </c>
       <c r="E385">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-3.0461302859137809</v>
       </c>
     </row>
@@ -19179,7 +19192,7 @@
         <v>-3.0292215188051226</v>
       </c>
       <c r="E386">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-3.0580467721911861</v>
       </c>
     </row>
@@ -19194,11 +19207,11 @@
         <v>-2.9012413748128001</v>
       </c>
       <c r="D387">
-        <f t="shared" ref="D387:D450" si="13">IF(B387&gt;$J$7,$I$2*SIN($I$3*B387+$I$5)+$I$4,$I$9*SIN($I$10*B387+$I$12)+$I$11)</f>
+        <f t="shared" ref="D387:D450" si="12">IF(B387&gt;($J$7+$M$2),$I$2*SIN($I$3*B387+($I$5-$M$2))+$I$4,$I$9*SIN($I$10*B387+($I$12-$M$2))+$I$11)</f>
         <v>-3.040119043994141</v>
       </c>
       <c r="E387">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="E387:E450" si="13">IF(B387&gt;($J$7+$M$2),$J$2*(B387+($J$5-$M$2))^2+$J$4,$J$9*(B387+($J$12-$M$2))^2+$J$11)</f>
         <v>-3.0697591647973277</v>
       </c>
     </row>
@@ -19213,11 +19226,11 @@
         <v>-2.9122503893053602</v>
       </c>
       <c r="D388">
+        <f t="shared" si="12"/>
+        <v>-3.0506632061530135</v>
+      </c>
+      <c r="E388">
         <f t="shared" si="13"/>
-        <v>-3.0506632061530135</v>
-      </c>
-      <c r="E388">
-        <f t="shared" si="12"/>
         <v>-3.0812674637322175</v>
       </c>
     </row>
@@ -19232,11 +19245,11 @@
         <v>-2.9230059014277598</v>
       </c>
       <c r="D389">
+        <f t="shared" si="12"/>
+        <v>-3.060853202302964</v>
+      </c>
+      <c r="E389">
         <f t="shared" si="13"/>
-        <v>-3.060853202302964</v>
-      </c>
-      <c r="E389">
-        <f t="shared" si="12"/>
         <v>-3.0925716689958502</v>
       </c>
     </row>
@@ -19251,11 +19264,11 @@
         <v>-2.9335085584901801</v>
       </c>
       <c r="D390">
+        <f t="shared" si="12"/>
+        <v>-3.0706882564363416</v>
+      </c>
+      <c r="E390">
         <f t="shared" si="13"/>
-        <v>-3.0706882564363416</v>
-      </c>
-      <c r="E390">
-        <f t="shared" si="12"/>
         <v>-3.1036717805882388</v>
       </c>
     </row>
@@ -19270,11 +19283,11 @@
         <v>-2.9437590435183401</v>
       </c>
       <c r="D391">
+        <f t="shared" si="12"/>
+        <v>-3.0801676195756769</v>
+      </c>
+      <c r="E391">
         <f t="shared" si="13"/>
-        <v>-3.0801676195756769</v>
-      </c>
-      <c r="E391">
-        <f t="shared" si="12"/>
         <v>-3.1145677985093574</v>
       </c>
     </row>
@@ -19289,11 +19302,11 @@
         <v>-2.9537580756631701</v>
       </c>
       <c r="D392">
+        <f t="shared" si="12"/>
+        <v>-3.0892905698307742</v>
+      </c>
+      <c r="E392">
         <f t="shared" si="13"/>
-        <v>-3.0892905698307742</v>
-      </c>
-      <c r="E392">
-        <f t="shared" si="12"/>
         <v>-3.1252597227592194</v>
       </c>
     </row>
@@ -19308,11 +19321,11 @@
         <v>-2.9635064106190399</v>
       </c>
       <c r="D393">
+        <f t="shared" si="12"/>
+        <v>-3.0980564124536536</v>
+      </c>
+      <c r="E393">
         <f t="shared" si="13"/>
-        <v>-3.0980564124536536</v>
-      </c>
-      <c r="E393">
-        <f t="shared" si="12"/>
         <v>-3.1357475533378238</v>
       </c>
     </row>
@@ -19327,11 +19340,11 @@
         <v>-2.9730048410521701</v>
       </c>
       <c r="D394">
+        <f t="shared" si="12"/>
+        <v>-3.1064644798914602</v>
+      </c>
+      <c r="E394">
         <f t="shared" si="13"/>
-        <v>-3.1064644798914602</v>
-      </c>
-      <c r="E394">
-        <f t="shared" si="12"/>
         <v>-3.1460312902451713</v>
       </c>
     </row>
@@ -19346,11 +19359,11 @@
         <v>-2.98225419703701</v>
       </c>
       <c r="D395">
+        <f t="shared" si="12"/>
+        <v>-3.1145141318373049</v>
+      </c>
+      <c r="E395">
         <f t="shared" si="13"/>
-        <v>-3.1145141318373049</v>
-      </c>
-      <c r="E395">
-        <f t="shared" si="12"/>
         <v>-3.1561109334812616</v>
       </c>
     </row>
@@ -19365,11 +19378,11 @@
         <v>-2.9912553465031002</v>
       </c>
       <c r="D396">
+        <f t="shared" si="12"/>
+        <v>-3.1222047552790344</v>
+      </c>
+      <c r="E396">
         <f t="shared" si="13"/>
-        <v>-3.1222047552790344</v>
-      </c>
-      <c r="E396">
-        <f t="shared" si="12"/>
         <v>-3.1659864830461064</v>
       </c>
     </row>
@@ -19384,11 +19397,11 @@
         <v>-3.0000091956907302</v>
       </c>
       <c r="D397">
+        <f t="shared" si="12"/>
+        <v>-3.1295357645458819</v>
+      </c>
+      <c r="E397">
         <f t="shared" si="13"/>
-        <v>-3.1295357645458819</v>
-      </c>
-      <c r="E397">
-        <f t="shared" si="12"/>
         <v>-3.1756579389396826</v>
       </c>
     </row>
@@ -19403,11 +19416,11 @@
         <v>-3.0085166896161</v>
       </c>
       <c r="D398">
+        <f t="shared" si="12"/>
+        <v>-3.1365066013531169</v>
+      </c>
+      <c r="E398">
         <f t="shared" si="13"/>
-        <v>-3.1365066013531169</v>
-      </c>
-      <c r="E398">
-        <f t="shared" si="12"/>
         <v>-3.1851253011620018</v>
       </c>
     </row>
@@ -19422,11 +19435,11 @@
         <v>-3.0167788125466402</v>
       </c>
       <c r="D399">
+        <f t="shared" si="12"/>
+        <v>-3.1431167348445279</v>
+      </c>
+      <c r="E399">
         <f t="shared" si="13"/>
-        <v>-3.1431167348445279</v>
-      </c>
-      <c r="E399">
-        <f t="shared" si="12"/>
         <v>-3.1943885697130643</v>
       </c>
     </row>
@@ -19441,11 +19454,11 @@
         <v>-3.0247965884857702</v>
       </c>
       <c r="D400">
+        <f t="shared" si="12"/>
+        <v>-3.1493656616328587</v>
+      </c>
+      <c r="E400">
         <f t="shared" si="13"/>
-        <v>-3.1493656616328587</v>
-      </c>
-      <c r="E400">
-        <f t="shared" si="12"/>
         <v>-3.2034477445928693</v>
       </c>
     </row>
@@ -19460,11 +19473,11 @@
         <v>-3.0325710816672302</v>
       </c>
       <c r="D401">
+        <f t="shared" si="12"/>
+        <v>-3.1552529058381382</v>
+      </c>
+      <c r="E401">
         <f t="shared" si="13"/>
-        <v>-3.1552529058381382</v>
-      </c>
-      <c r="E401">
-        <f t="shared" si="12"/>
         <v>-3.2123028258014177</v>
       </c>
     </row>
@@ -19479,11 +19492,11 @@
         <v>-3.0401033970603999</v>
       </c>
       <c r="D402">
+        <f t="shared" si="12"/>
+        <v>-3.1607780191239283</v>
+      </c>
+      <c r="E402">
         <f t="shared" si="13"/>
-        <v>-3.1607780191239283</v>
-      </c>
-      <c r="E402">
-        <f t="shared" si="12"/>
         <v>-3.2209538133387086</v>
       </c>
     </row>
@@ -19498,11 +19511,11 @@
         <v>-3.0473946808841901</v>
       </c>
       <c r="D403">
+        <f t="shared" si="12"/>
+        <v>-3.1659405807314669</v>
+      </c>
+      <c r="E403">
         <f t="shared" si="13"/>
-        <v>-3.1659405807314669</v>
-      </c>
-      <c r="E403">
-        <f t="shared" si="12"/>
         <v>-3.2294007072047526</v>
       </c>
     </row>
@@ -19517,11 +19530,11 @@
         <v>-3.0544461211323899</v>
       </c>
       <c r="D404">
+        <f t="shared" si="12"/>
+        <v>-3.1707401975116878</v>
+      </c>
+      <c r="E404">
         <f t="shared" si="13"/>
-        <v>-3.1707401975116878</v>
-      </c>
-      <c r="E404">
-        <f t="shared" si="12"/>
         <v>-3.2376435073995293</v>
       </c>
     </row>
@@ -19536,11 +19549,11 @@
         <v>-3.0612589481081698</v>
       </c>
       <c r="D405">
+        <f t="shared" si="12"/>
+        <v>-3.1751765039551958</v>
+      </c>
+      <c r="E405">
         <f t="shared" si="13"/>
-        <v>-3.1751765039551958</v>
-      </c>
-      <c r="E405">
-        <f t="shared" si="12"/>
         <v>-3.245682213923049</v>
       </c>
     </row>
@@ -19555,11 +19568,11 @@
         <v>-3.0678344349696598</v>
       </c>
       <c r="D406">
+        <f t="shared" si="12"/>
+        <v>-3.1792491622200809</v>
+      </c>
+      <c r="E406">
         <f t="shared" si="13"/>
-        <v>-3.1792491622200809</v>
-      </c>
-      <c r="E406">
-        <f t="shared" si="12"/>
         <v>-3.2535168267753121</v>
       </c>
     </row>
@@ -19574,11 +19587,11 @@
         <v>-3.07417389828495</v>
       </c>
       <c r="D407">
+        <f t="shared" si="12"/>
+        <v>-3.1829578621576471</v>
+      </c>
+      <c r="E407">
         <f t="shared" si="13"/>
-        <v>-3.1829578621576471</v>
-      </c>
-      <c r="E407">
-        <f t="shared" si="12"/>
         <v>-3.2611473459563176</v>
       </c>
     </row>
@@ -19593,11 +19606,11 @@
         <v>-3.0802786985983901</v>
       </c>
       <c r="D408">
+        <f t="shared" si="12"/>
+        <v>-3.1863023213360351</v>
+      </c>
+      <c r="E408">
         <f t="shared" si="13"/>
-        <v>-3.1863023213360351</v>
-      </c>
-      <c r="E408">
-        <f t="shared" si="12"/>
         <v>-3.2685737714660665</v>
       </c>
     </row>
@@ -19612,11 +19625,11 @@
         <v>-3.0861502410060502</v>
       </c>
       <c r="D409">
+        <f t="shared" si="12"/>
+        <v>-3.1892822850617351</v>
+      </c>
+      <c r="E409">
         <f t="shared" si="13"/>
-        <v>-3.1892822850617351</v>
-      </c>
-      <c r="E409">
-        <f t="shared" si="12"/>
         <v>-3.2757961033045664</v>
       </c>
     </row>
@@ -19631,11 +19644,11 @@
         <v>-3.0917899757426399</v>
       </c>
       <c r="D410">
+        <f t="shared" si="12"/>
+        <v>-3.1918975263989631</v>
+      </c>
+      <c r="E410">
         <f t="shared" si="13"/>
-        <v>-3.1918975263989631</v>
-      </c>
-      <c r="E410">
-        <f t="shared" si="12"/>
         <v>-3.2828143414718012</v>
       </c>
     </row>
@@ -19650,11 +19663,11 @@
         <v>-3.0971993987781001</v>
       </c>
       <c r="D411">
+        <f t="shared" si="12"/>
+        <v>-3.1941478461869708</v>
+      </c>
+      <c r="E411">
         <f t="shared" si="13"/>
-        <v>-3.1941478461869708</v>
-      </c>
-      <c r="E411">
-        <f t="shared" si="12"/>
         <v>-3.2896284859677785</v>
       </c>
     </row>
@@ -19669,11 +19682,11 @@
         <v>-3.10238005242479</v>
       </c>
       <c r="D412">
+        <f t="shared" si="12"/>
+        <v>-3.1960330730551934</v>
+      </c>
+      <c r="E412">
         <f t="shared" si="13"/>
-        <v>-3.1960330730551934</v>
-      </c>
-      <c r="E412">
-        <f t="shared" si="12"/>
         <v>-3.2962385367924991</v>
       </c>
     </row>
@@ -19688,11 +19701,11 @@
         <v>-3.1073335259548198</v>
       </c>
       <c r="D413">
+        <f t="shared" si="12"/>
+        <v>-3.1975530634363056</v>
+      </c>
+      <c r="E413">
         <f t="shared" si="13"/>
-        <v>-3.1975530634363056</v>
-      </c>
-      <c r="E413">
-        <f t="shared" si="12"/>
         <v>-3.3026444939459627</v>
       </c>
     </row>
@@ -19707,11 +19720,11 @@
         <v>-3.11206145622796</v>
       </c>
       <c r="D414">
+        <f t="shared" si="12"/>
+        <v>-3.1987077015771557</v>
+      </c>
+      <c r="E414">
         <f t="shared" si="13"/>
-        <v>-3.1987077015771557</v>
-      </c>
-      <c r="E414">
-        <f t="shared" si="12"/>
         <v>-3.3088463574281692</v>
       </c>
     </row>
@@ -19726,11 +19739,11 @@
         <v>-3.1165655283290201</v>
       </c>
       <c r="D415">
+        <f t="shared" si="12"/>
+        <v>-3.199496899547579</v>
+      </c>
+      <c r="E415">
         <f t="shared" si="13"/>
-        <v>-3.199496899547579</v>
-      </c>
-      <c r="E415">
-        <f t="shared" si="12"/>
         <v>-3.3148441272391254</v>
       </c>
     </row>
@@ -19745,11 +19758,11 @@
         <v>-3.1208474762163898</v>
       </c>
       <c r="D416">
+        <f t="shared" si="12"/>
+        <v>-3.1999205972470928</v>
+      </c>
+      <c r="E416">
         <f t="shared" si="13"/>
-        <v>-3.1999205972470928</v>
-      </c>
-      <c r="E416">
-        <f t="shared" si="12"/>
         <v>-3.3206378033788178</v>
       </c>
     </row>
@@ -19764,11 +19777,11 @@
         <v>-3.1249090833795599</v>
       </c>
       <c r="D417">
+        <f t="shared" si="12"/>
+        <v>-3.199978762409478</v>
+      </c>
+      <c r="E417">
         <f t="shared" si="13"/>
-        <v>-3.199978762409478</v>
-      </c>
-      <c r="E417">
-        <f t="shared" si="12"/>
         <v>-3.3262273858472526</v>
       </c>
     </row>
@@ -19783,11 +19796,11 @@
         <v>-3.12875218350701</v>
       </c>
       <c r="D418">
+        <f t="shared" si="12"/>
+        <v>-3.1996713906052334</v>
+      </c>
+      <c r="E418">
         <f t="shared" si="13"/>
-        <v>-3.1996713906052334</v>
-      </c>
-      <c r="E418">
-        <f t="shared" si="12"/>
         <v>-3.3316128746444309</v>
       </c>
     </row>
@@ -19802,11 +19815,11 @@
         <v>-3.1323786611637598</v>
       </c>
       <c r="D419">
+        <f t="shared" si="12"/>
+        <v>-3.1989985052419105</v>
+      </c>
+      <c r="E419">
         <f t="shared" si="13"/>
-        <v>-3.1989985052419105</v>
-      </c>
-      <c r="E419">
-        <f t="shared" si="12"/>
         <v>-3.3367942697703521</v>
       </c>
     </row>
@@ -19821,11 +19834,11 @@
         <v>-3.1357904524784299</v>
       </c>
       <c r="D420">
+        <f t="shared" si="12"/>
+        <v>-3.1979601575623353</v>
+      </c>
+      <c r="E420">
         <f t="shared" si="13"/>
-        <v>-3.1979601575623353</v>
-      </c>
-      <c r="E420">
-        <f t="shared" si="12"/>
         <v>-3.3417715712250162</v>
       </c>
     </row>
@@ -19840,11 +19853,11 @@
         <v>-3.13898954583926</v>
       </c>
       <c r="D421">
+        <f t="shared" si="12"/>
+        <v>-3.1965564266407038</v>
+      </c>
+      <c r="E421">
         <f t="shared" si="13"/>
-        <v>-3.1965564266407038</v>
-      </c>
-      <c r="E421">
-        <f t="shared" si="12"/>
         <v>-3.3465447790084233</v>
       </c>
     </row>
@@ -19859,11 +19872,11 @@
         <v>-3.14197798259974</v>
       </c>
       <c r="D422">
+        <f t="shared" si="12"/>
+        <v>-3.1947874193765577</v>
+      </c>
+      <c r="E422">
         <f t="shared" si="13"/>
-        <v>-3.1947874193765577</v>
-      </c>
-      <c r="E422">
-        <f t="shared" si="12"/>
         <v>-3.3511138931205786</v>
       </c>
     </row>
@@ -19878,11 +19891,11 @@
         <v>-3.1447578577925701</v>
       </c>
       <c r="D423">
+        <f t="shared" si="12"/>
+        <v>-3.1926532704866548</v>
+      </c>
+      <c r="E423">
         <f t="shared" si="13"/>
-        <v>-3.1926532704866548</v>
-      </c>
-      <c r="E423">
-        <f t="shared" si="12"/>
         <v>-3.3554789135614715</v>
       </c>
     </row>
@@ -19897,11 +19910,11 @@
         <v>-3.1473313208524498</v>
       </c>
       <c r="D424">
+        <f t="shared" si="12"/>
+        <v>-3.1901541424946926</v>
+      </c>
+      <c r="E424">
         <f t="shared" si="13"/>
-        <v>-3.1901541424946926</v>
-      </c>
-      <c r="E424">
-        <f t="shared" si="12"/>
         <v>-3.3596398403311074</v>
       </c>
     </row>
@@ -19916,11 +19929,11 @@
         <v>-3.1497005763465098</v>
       </c>
       <c r="D425">
+        <f t="shared" si="12"/>
+        <v>-3.1872902257189435</v>
+      </c>
+      <c r="E425">
         <f t="shared" si="13"/>
-        <v>-3.1872902257189435</v>
-      </c>
-      <c r="E425">
-        <f t="shared" si="12"/>
         <v>-3.3635966734294862</v>
       </c>
     </row>
@@ -19935,11 +19948,11 @@
         <v>-3.1518678847130599</v>
       </c>
       <c r="D426">
+        <f t="shared" si="12"/>
+        <v>-3.1840617382577583</v>
+      </c>
+      <c r="E426">
         <f t="shared" si="13"/>
-        <v>-3.1840617382577583</v>
-      </c>
-      <c r="E426">
-        <f t="shared" si="12"/>
         <v>-3.3673494128566079</v>
       </c>
     </row>
@@ -19954,11 +19967,11 @@
         <v>-3.1538355630070898</v>
       </c>
       <c r="D427">
+        <f t="shared" si="12"/>
+        <v>-3.1804689259729568</v>
+      </c>
+      <c r="E427">
         <f t="shared" si="13"/>
-        <v>-3.1804689259729568</v>
-      </c>
-      <c r="E427">
-        <f t="shared" ref="E427:E490" si="14">IF(B427&gt;$J$7,$J$2*(B427+$J$5)^2+$J$4,$J$9*(B427+$J$12)^2+$J$11)</f>
         <v>-3.370898058612473</v>
       </c>
     </row>
@@ -19973,11 +19986,11 @@
         <v>-3.1556059856533198</v>
       </c>
       <c r="D428">
+        <f t="shared" si="12"/>
+        <v>-3.1765120624710996</v>
+      </c>
+      <c r="E428">
         <f t="shared" si="13"/>
-        <v>-3.1765120624710996</v>
-      </c>
-      <c r="E428">
-        <f t="shared" si="14"/>
         <v>-3.3742426106970842</v>
       </c>
     </row>
@@ -19992,11 +20005,11 @@
         <v>-3.15718158520454</v>
       </c>
       <c r="D429">
+        <f t="shared" si="12"/>
+        <v>-3.1721914490826708</v>
+      </c>
+      <c r="E429">
         <f t="shared" si="13"/>
-        <v>-3.1721914490826708</v>
-      </c>
-      <c r="E429">
-        <f t="shared" si="14"/>
         <v>-3.3773830691104347</v>
       </c>
     </row>
@@ -20011,11 +20024,11 @@
         <v>-3.1585648531066601</v>
       </c>
       <c r="D430">
+        <f t="shared" si="12"/>
+        <v>-3.1675074148391045</v>
+      </c>
+      <c r="E430">
         <f t="shared" si="13"/>
-        <v>-3.1675074148391045</v>
-      </c>
-      <c r="E430">
-        <f t="shared" si="14"/>
         <v>-3.3803194338525282</v>
       </c>
     </row>
@@ -20030,11 +20043,11 @@
         <v>-3.1597583404684202</v>
       </c>
       <c r="D431">
+        <f t="shared" si="12"/>
+        <v>-3.1624603164477434</v>
+      </c>
+      <c r="E431">
         <f t="shared" si="13"/>
-        <v>-3.1624603164477434</v>
-      </c>
-      <c r="E431">
-        <f t="shared" si="14"/>
         <v>-3.383051704923365</v>
       </c>
     </row>
@@ -20049,11 +20062,11 @@
         <v>-3.1607646588357801</v>
       </c>
       <c r="D432">
+        <f t="shared" si="12"/>
+        <v>-3.1570505382646705</v>
+      </c>
+      <c r="E432">
         <f t="shared" si="13"/>
-        <v>-3.1570505382646705</v>
-      </c>
-      <c r="E432">
-        <f t="shared" si="14"/>
         <v>-3.3855798823229444</v>
       </c>
     </row>
@@ -20068,11 +20081,11 @@
         <v>-3.1615864809692802</v>
       </c>
       <c r="D433">
+        <f t="shared" si="12"/>
+        <v>-3.1512784922654382</v>
+      </c>
+      <c r="E433">
         <f t="shared" si="13"/>
-        <v>-3.1512784922654382</v>
-      </c>
-      <c r="E433">
-        <f t="shared" si="14"/>
         <v>-3.3879039660512666</v>
       </c>
     </row>
@@ -20087,11 +20100,11 @@
         <v>-3.1622265416256901</v>
       </c>
       <c r="D434">
+        <f t="shared" si="12"/>
+        <v>-3.1451446180136968</v>
+      </c>
+      <c r="E434">
         <f t="shared" si="13"/>
-        <v>-3.1451446180136968</v>
-      </c>
-      <c r="E434">
-        <f t="shared" si="14"/>
         <v>-3.3900239561083323</v>
       </c>
     </row>
@@ -20106,11 +20119,11 @@
         <v>-3.1626876383404099</v>
       </c>
       <c r="D435">
+        <f t="shared" si="12"/>
+        <v>-3.1386493826277122</v>
+      </c>
+      <c r="E435">
         <f t="shared" si="13"/>
-        <v>-3.1386493826277122</v>
-      </c>
-      <c r="E435">
-        <f t="shared" si="14"/>
         <v>-3.3919398524941426</v>
       </c>
     </row>
@@ -20125,11 +20138,11 @@
         <v>-3.16297263221146</v>
       </c>
       <c r="D436">
+        <f t="shared" si="12"/>
+        <v>-3.1317932807448217</v>
+      </c>
+      <c r="E436">
         <f t="shared" si="13"/>
-        <v>-3.1317932807448217</v>
-      </c>
-      <c r="E436">
-        <f t="shared" si="14"/>
         <v>-3.3936516552086937</v>
       </c>
     </row>
@@ -20144,11 +20157,11 @@
         <v>-3.16308444868372</v>
       </c>
       <c r="D437">
+        <f t="shared" si="12"/>
+        <v>-3.1245768344837193</v>
+      </c>
+      <c r="E437">
         <f t="shared" si="13"/>
-        <v>-3.1245768344837193</v>
-      </c>
-      <c r="E437">
-        <f t="shared" si="14"/>
         <v>-3.3951593642519882</v>
       </c>
     </row>
@@ -20163,11 +20176,11 @@
         <v>-3.1630260783319999</v>
       </c>
       <c r="D438">
+        <f t="shared" si="12"/>
+        <v>-3.1170005934047276</v>
+      </c>
+      <c r="E438">
         <f t="shared" si="13"/>
-        <v>-3.1170005934047276</v>
-      </c>
-      <c r="E438">
-        <f t="shared" si="14"/>
         <v>-3.3964629796240251</v>
       </c>
     </row>
@@ -20182,11 +20195,11 @@
         <v>-3.1628005776415802</v>
       </c>
       <c r="D439">
+        <f t="shared" si="12"/>
+        <v>-3.1090651344679379</v>
+      </c>
+      <c r="E439">
         <f t="shared" si="13"/>
-        <v>-3.1090651344679379</v>
-      </c>
-      <c r="E439">
-        <f t="shared" si="14"/>
         <v>-3.3975625013248054</v>
       </c>
     </row>
@@ -20201,11 +20214,11 @@
         <v>-3.1624110697864198</v>
       </c>
       <c r="D440">
+        <f t="shared" si="12"/>
+        <v>-3.1007710619892719</v>
+      </c>
+      <c r="E440">
         <f t="shared" si="13"/>
-        <v>-3.1007710619892719</v>
-      </c>
-      <c r="E440">
-        <f t="shared" si="14"/>
         <v>-3.3984579293543282</v>
       </c>
     </row>
@@ -20220,11 +20233,11 @@
         <v>-3.16186074540088</v>
       </c>
       <c r="D441">
+        <f t="shared" si="12"/>
+        <v>-3.0921190075944511</v>
+      </c>
+      <c r="E441">
         <f t="shared" si="13"/>
-        <v>-3.0921190075944511</v>
-      </c>
-      <c r="E441">
-        <f t="shared" si="14"/>
         <v>-3.3991492637125948</v>
       </c>
     </row>
@@ -20239,11 +20252,11 @@
         <v>-3.1611528633474002</v>
       </c>
       <c r="D442">
+        <f t="shared" si="12"/>
+        <v>-3.0831096301709349</v>
+      </c>
+      <c r="E442">
         <f t="shared" si="13"/>
-        <v>-3.0831096301709349</v>
-      </c>
-      <c r="E442">
-        <f t="shared" si="14"/>
         <v>-3.399636504399604</v>
       </c>
     </row>
@@ -20258,11 +20271,11 @@
         <v>-3.1602907514741498</v>
       </c>
       <c r="D443">
+        <f t="shared" si="12"/>
+        <v>-3.073743615817683</v>
+      </c>
+      <c r="E443">
         <f t="shared" si="13"/>
-        <v>-3.073743615817683</v>
-      </c>
-      <c r="E443">
-        <f t="shared" si="14"/>
         <v>-3.3999196514153556</v>
       </c>
     </row>
@@ -20277,11 +20290,11 @@
         <v>-3.1592778073653101</v>
       </c>
       <c r="D444">
+        <f t="shared" si="12"/>
+        <v>-3.0640216777929532</v>
+      </c>
+      <c r="E444">
         <f t="shared" si="13"/>
-        <v>-3.0640216777929532</v>
-      </c>
-      <c r="E444">
-        <f t="shared" si="14"/>
         <v>-3.3999987047598506</v>
       </c>
     </row>
@@ -20296,11 +20309,11 @@
         <v>-3.1581174990788501</v>
       </c>
       <c r="D445">
+        <f t="shared" si="12"/>
+        <v>-3.053944556459967</v>
+      </c>
+      <c r="E445">
         <f t="shared" si="13"/>
-        <v>-3.053944556459967</v>
-      </c>
-      <c r="E445">
-        <f t="shared" si="14"/>
         <v>-3.399873664433088</v>
       </c>
     </row>
@@ -20315,11 +20328,11 @@
         <v>-3.1568133658719701</v>
       </c>
       <c r="D446">
+        <f t="shared" si="12"/>
+        <v>-3.0435130192305269</v>
+      </c>
+      <c r="E446">
         <f t="shared" si="13"/>
-        <v>-3.0435130192305269</v>
-      </c>
-      <c r="E446">
-        <f t="shared" si="14"/>
         <v>-3.3995445304350689</v>
       </c>
     </row>
@@ -20334,11 +20347,11 @@
         <v>-3.1553690189118702</v>
       </c>
       <c r="D447">
+        <f t="shared" si="12"/>
+        <v>-3.0327278605065797</v>
+      </c>
+      <c r="E447">
         <f t="shared" si="13"/>
-        <v>-3.0327278605065797</v>
-      </c>
-      <c r="E447">
-        <f t="shared" si="14"/>
         <v>-3.3990113027657927</v>
       </c>
     </row>
@@ -20353,11 +20366,11 @@
         <v>-3.15378814196841</v>
       </c>
       <c r="D448">
+        <f t="shared" si="12"/>
+        <v>-3.0215899016197079</v>
+      </c>
+      <c r="E448">
         <f t="shared" si="13"/>
-        <v>-3.0215899016197079</v>
-      </c>
-      <c r="E448">
-        <f t="shared" si="14"/>
         <v>-3.3982739814252585</v>
       </c>
     </row>
@@ -20372,11 +20385,11 @@
         <v>-3.1520744920890298</v>
       </c>
       <c r="D449">
+        <f t="shared" si="12"/>
+        <v>-3.0100999907686261</v>
+      </c>
+      <c r="E449">
         <f t="shared" si="13"/>
-        <v>-3.0100999907686261</v>
-      </c>
-      <c r="E449">
-        <f t="shared" si="14"/>
         <v>-3.3973325664134681</v>
       </c>
     </row>
@@ -20391,11 +20404,11 @@
         <v>-3.1502319002506698</v>
       </c>
       <c r="D450">
+        <f t="shared" si="12"/>
+        <v>-2.9982590029545206</v>
+      </c>
+      <c r="E450">
         <f t="shared" si="13"/>
-        <v>-2.9982590029545206</v>
-      </c>
-      <c r="E450">
-        <f t="shared" si="14"/>
         <v>-3.3961870577304203</v>
       </c>
     </row>
@@ -20410,11 +20423,11 @@
         <v>-3.1482642719889302</v>
       </c>
       <c r="D451">
-        <f t="shared" ref="D451:D514" si="15">IF(B451&gt;$J$7,$I$2*SIN($I$3*B451+$I$5)+$I$4,$I$9*SIN($I$10*B451+$I$12)+$I$11)</f>
+        <f t="shared" ref="D451:D514" si="14">IF(B451&gt;($J$7+$M$2),$I$2*SIN($I$3*B451+($I$5-$M$2))+$I$4,$I$9*SIN($I$10*B451+($I$12-$M$2))+$I$11)</f>
         <v>-2.9860678399144578</v>
       </c>
       <c r="E451">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="E451:E514" si="15">IF(B451&gt;($J$7+$M$2),$J$2*(B451+($J$5-$M$2))^2+$J$4,$J$9*(B451+($J$12-$M$2))^2+$J$11)</f>
         <v>-3.3948374553761158</v>
       </c>
     </row>
@@ -20429,11 +20442,11 @@
         <v>-3.1461755879995899</v>
       </c>
       <c r="D452">
+        <f t="shared" si="14"/>
+        <v>-2.9735274300527013</v>
+      </c>
+      <c r="E452">
         <f t="shared" si="15"/>
-        <v>-2.9735274300527013</v>
-      </c>
-      <c r="E452">
-        <f t="shared" si="14"/>
         <v>-3.3932837593505543</v>
       </c>
     </row>
@@ -20448,11 +20461,11 @@
         <v>-3.1439699047114402</v>
       </c>
       <c r="D453">
+        <f t="shared" si="14"/>
+        <v>-2.960638728370014</v>
+      </c>
+      <c r="E453">
         <f t="shared" si="15"/>
-        <v>-2.960638728370014</v>
-      </c>
-      <c r="E453">
-        <f t="shared" si="14"/>
         <v>-3.3915259696537357</v>
       </c>
     </row>
@@ -20467,11 +20480,11 @@
         <v>-3.1416513548265499</v>
       </c>
       <c r="D454">
+        <f t="shared" si="14"/>
+        <v>-2.9474027163909162</v>
+      </c>
+      <c r="E454">
         <f t="shared" si="15"/>
-        <v>-2.9474027163909162</v>
-      </c>
-      <c r="E454">
-        <f t="shared" si="14"/>
         <v>-3.3895640862856578</v>
       </c>
     </row>
@@ -20486,11 +20499,11 @@
         <v>-3.1392241478249199</v>
       </c>
       <c r="D455">
+        <f t="shared" si="14"/>
+        <v>-2.9338204020889944</v>
+      </c>
+      <c r="E455">
         <f t="shared" si="15"/>
-        <v>-2.9338204020889944</v>
-      </c>
-      <c r="E455">
-        <f t="shared" si="14"/>
         <v>-3.3873981092463246</v>
       </c>
     </row>
@@ -20505,11 +20518,11 @@
         <v>-3.13669257043163</v>
       </c>
       <c r="D456">
+        <f t="shared" si="14"/>
+        <v>-2.919892819810054</v>
+      </c>
+      <c r="E456">
         <f t="shared" si="15"/>
-        <v>-2.919892819810054</v>
-      </c>
-      <c r="E456">
-        <f t="shared" si="14"/>
         <v>-3.3850280385357348</v>
       </c>
     </row>
@@ -20524,11 +20537,11 @@
         <v>-3.1340609870413401</v>
       </c>
       <c r="D457">
+        <f t="shared" si="14"/>
+        <v>-2.90562103019341</v>
+      </c>
+      <c r="E457">
         <f t="shared" si="15"/>
-        <v>-2.90562103019341</v>
-      </c>
-      <c r="E457">
-        <f t="shared" si="14"/>
         <v>-3.3824538741538879</v>
       </c>
     </row>
@@ -20543,11 +20556,11 @@
         <v>-3.1313338400979598</v>
       </c>
       <c r="D458">
+        <f t="shared" si="14"/>
+        <v>-2.8910061200910948</v>
+      </c>
+      <c r="E458">
         <f t="shared" si="15"/>
-        <v>-2.8910061200910948</v>
-      </c>
-      <c r="E458">
-        <f t="shared" si="14"/>
         <v>-3.3796756161007839</v>
       </c>
     </row>
@@ -20562,11 +20575,11 @@
         <v>-3.1285156504248501</v>
       </c>
       <c r="D459">
+        <f t="shared" si="14"/>
+        <v>-2.8760492024850977</v>
+      </c>
+      <c r="E459">
         <f t="shared" si="15"/>
-        <v>-2.8760492024850977</v>
-      </c>
-      <c r="E459">
-        <f t="shared" si="14"/>
         <v>-3.3766932643764229</v>
       </c>
     </row>
@@ -20581,11 +20594,11 @@
         <v>-3.12561101750343</v>
       </c>
       <c r="D460">
+        <f t="shared" si="14"/>
+        <v>-2.8607514164026031</v>
+      </c>
+      <c r="E460">
         <f t="shared" si="15"/>
-        <v>-2.8607514164026031</v>
-      </c>
-      <c r="E460">
-        <f t="shared" si="14"/>
         <v>-3.3735068189808053</v>
       </c>
     </row>
@@ -20600,11 +20613,11 @@
         <v>-3.12262461969389</v>
       </c>
       <c r="D461">
+        <f t="shared" si="14"/>
+        <v>-2.8451139268292303</v>
+      </c>
+      <c r="E461">
         <f t="shared" si="15"/>
-        <v>-2.8451139268292303</v>
-      </c>
-      <c r="E461">
-        <f t="shared" si="14"/>
         <v>-3.3701162799139261</v>
       </c>
     </row>
@@ -20619,11 +20632,11 @@
         <v>-3.1195612143962599</v>
       </c>
       <c r="D462">
+        <f t="shared" si="14"/>
+        <v>-2.8291379246203872</v>
+      </c>
+      <c r="E462">
         <f t="shared" si="15"/>
-        <v>-2.8291379246203872</v>
-      </c>
-      <c r="E462">
-        <f t="shared" si="14"/>
         <v>-3.3665216471757939</v>
       </c>
     </row>
@@ -20638,11 +20651,11 @@
         <v>-3.1164256381456501</v>
       </c>
       <c r="D463">
+        <f t="shared" si="14"/>
+        <v>-2.8128246264104804</v>
+      </c>
+      <c r="E463">
         <f t="shared" si="15"/>
-        <v>-2.8128246264104804</v>
-      </c>
-      <c r="E463">
-        <f t="shared" si="14"/>
         <v>-3.3627229207664047</v>
       </c>
     </row>
@@ -20657,11 +20670,11 @@
         <v>-3.11322280663873</v>
       </c>
       <c r="D464">
+        <f t="shared" si="14"/>
+        <v>-2.7961752745203268</v>
+      </c>
+      <c r="E464">
         <f t="shared" si="15"/>
-        <v>-2.7961752745203268</v>
-      </c>
-      <c r="E464">
-        <f t="shared" si="14"/>
         <v>-3.3587201006857583</v>
       </c>
     </row>
@@ -20676,11 +20689,11 @@
         <v>-3.1099577146858302</v>
       </c>
       <c r="D465">
+        <f t="shared" si="14"/>
+        <v>-2.779191136862535</v>
+      </c>
+      <c r="E465">
         <f t="shared" si="15"/>
-        <v>-2.779191136862535</v>
-      </c>
-      <c r="E465">
-        <f t="shared" si="14"/>
         <v>-3.3545131869338549</v>
       </c>
     </row>
@@ -20695,11 +20708,11 @@
         <v>-3.10663543608496</v>
       </c>
       <c r="D466">
+        <f t="shared" si="14"/>
+        <v>-2.7618735068449438</v>
+      </c>
+      <c r="E466">
         <f t="shared" si="15"/>
-        <v>-2.7618735068449438</v>
-      </c>
-      <c r="E466">
-        <f t="shared" si="14"/>
         <v>-3.3501021795106949</v>
       </c>
     </row>
@@ -20714,11 +20727,11 @@
         <v>-3.1032611234116301</v>
       </c>
       <c r="D467">
+        <f t="shared" si="14"/>
+        <v>-2.7442237032721057</v>
+      </c>
+      <c r="E467">
         <f t="shared" si="15"/>
-        <v>-2.7442237032721057</v>
-      </c>
-      <c r="E467">
-        <f t="shared" si="14"/>
         <v>-3.345487078416272</v>
       </c>
     </row>
@@ -20733,11 +20746,11 @@
         <v>-3.0998400077207999</v>
       </c>
       <c r="D468">
+        <f t="shared" si="14"/>
+        <v>-2.7262430702449367</v>
+      </c>
+      <c r="E468">
         <f t="shared" si="15"/>
-        <v>-2.7262430702449367</v>
-      </c>
-      <c r="E468">
-        <f t="shared" si="14"/>
         <v>-3.3406678836505974</v>
       </c>
     </row>
@@ -20752,11 +20765,11 @@
         <v>-3.0963773981553202</v>
       </c>
       <c r="D469">
+        <f t="shared" si="14"/>
+        <v>-2.7079329770582379</v>
+      </c>
+      <c r="E469">
         <f t="shared" si="15"/>
-        <v>-2.7079329770582379</v>
-      </c>
-      <c r="E469">
-        <f t="shared" si="14"/>
         <v>-3.3356445952136657</v>
       </c>
     </row>
@@ -20771,11 +20784,11 @@
         <v>-3.0928786814553599</v>
       </c>
       <c r="D470">
+        <f t="shared" si="14"/>
+        <v>-2.689294818096498</v>
+      </c>
+      <c r="E470">
         <f t="shared" si="15"/>
-        <v>-2.689294818096498</v>
-      </c>
-      <c r="E470">
-        <f t="shared" si="14"/>
         <v>-3.3304172131054774</v>
       </c>
     </row>
@@ -20790,11 +20803,11 @@
         <v>-3.0893493213637599</v>
       </c>
       <c r="D471">
+        <f t="shared" si="14"/>
+        <v>-2.670330012727677</v>
+      </c>
+      <c r="E471">
         <f t="shared" si="15"/>
-        <v>-2.670330012727677</v>
-      </c>
-      <c r="E471">
-        <f t="shared" si="14"/>
         <v>-3.3249857373260316</v>
       </c>
     </row>
@@ -20809,11 +20822,11 @@
         <v>-3.0857948579227101</v>
       </c>
       <c r="D472">
+        <f t="shared" si="14"/>
+        <v>-2.6510400051951319</v>
+      </c>
+      <c r="E472">
         <f t="shared" si="15"/>
-        <v>-2.6510400051951319</v>
-      </c>
-      <c r="E472">
-        <f t="shared" si="14"/>
         <v>-3.3193501678753292</v>
       </c>
     </row>
@@ -20828,11 +20841,11 @@
         <v>-3.0822209066544302</v>
       </c>
       <c r="D473">
+        <f t="shared" si="14"/>
+        <v>-2.6314262645076218</v>
+      </c>
+      <c r="E473">
         <f t="shared" si="15"/>
-        <v>-2.6314262645076218</v>
-      </c>
-      <c r="E473">
-        <f t="shared" si="14"/>
         <v>-3.3135105047533693</v>
       </c>
     </row>
@@ -20847,11 +20860,11 @@
         <v>-3.0786331576221202</v>
       </c>
       <c r="D474">
+        <f t="shared" si="14"/>
+        <v>-2.6114902843274135</v>
+      </c>
+      <c r="E474">
         <f t="shared" si="15"/>
-        <v>-2.6114902843274135</v>
-      </c>
-      <c r="E474">
-        <f t="shared" si="14"/>
         <v>-3.3074667479601456</v>
       </c>
     </row>
@@ -20866,11 +20879,11 @@
         <v>-3.0750373743650701</v>
       </c>
       <c r="D475">
+        <f t="shared" si="14"/>
+        <v>-2.5912335828566282</v>
+      </c>
+      <c r="E475">
         <f t="shared" si="15"/>
-        <v>-2.5912335828566282</v>
-      </c>
-      <c r="E475">
-        <f t="shared" si="14"/>
         <v>-3.3012188974956715</v>
       </c>
     </row>
@@ -20885,11 +20898,11 @@
         <v>-3.0714393927013202</v>
       </c>
       <c r="D476">
+        <f t="shared" si="14"/>
+        <v>-2.570657702721491</v>
+      </c>
+      <c r="E476">
         <f t="shared" si="15"/>
-        <v>-2.570657702721491</v>
-      </c>
-      <c r="E476">
-        <f t="shared" si="14"/>
         <v>-3.2947669533599409</v>
       </c>
     </row>
@@ -20904,11 +20917,11 @@
         <v>-3.0678451193939602</v>
       </c>
       <c r="D477">
+        <f t="shared" si="14"/>
+        <v>-2.549764210854931</v>
+      </c>
+      <c r="E477">
         <f t="shared" si="15"/>
-        <v>-2.549764210854931</v>
-      </c>
-      <c r="E477">
-        <f t="shared" si="14"/>
         <v>-3.2881109155529527</v>
       </c>
     </row>
@@ -20923,11 +20936,11 @@
         <v>-3.06426053067432</v>
       </c>
       <c r="D478">
+        <f t="shared" si="14"/>
+        <v>-2.5285546983772487</v>
+      </c>
+      <c r="E478">
         <f t="shared" si="15"/>
-        <v>-2.5285546983772487</v>
-      </c>
-      <c r="E478">
-        <f t="shared" si="14"/>
         <v>-3.2812507840747078</v>
       </c>
     </row>
@@ -20942,11 +20955,11 @@
         <v>-3.0606916706165599</v>
       </c>
       <c r="D479">
+        <f t="shared" si="14"/>
+        <v>-2.5070307804749379</v>
+      </c>
+      <c r="E479">
         <f t="shared" si="15"/>
-        <v>-2.5070307804749379</v>
-      </c>
-      <c r="E479">
-        <f t="shared" si="14"/>
         <v>-3.2741865589252059</v>
       </c>
     </row>
@@ -20961,11 +20974,11 @@
         <v>-3.0571446493588899</v>
       </c>
       <c r="D480">
+        <f t="shared" si="14"/>
+        <v>-2.485194096277652</v>
+      </c>
+      <c r="E480">
         <f t="shared" si="15"/>
-        <v>-2.485194096277652</v>
-      </c>
-      <c r="E480">
-        <f t="shared" si="14"/>
         <v>-3.2669182401044385</v>
       </c>
     </row>
@@ -20980,11 +20993,11 @@
         <v>-3.0536256411655698</v>
       </c>
       <c r="D481">
+        <f t="shared" si="14"/>
+        <v>-2.4630463087334857</v>
+      </c>
+      <c r="E481">
         <f t="shared" si="15"/>
-        <v>-2.4630463087334857</v>
-      </c>
-      <c r="E481">
-        <f t="shared" si="14"/>
         <v>-3.2594458276124221</v>
       </c>
     </row>
@@ -20999,11 +21012,11 @@
         <v>-3.0501408823244698</v>
       </c>
       <c r="D482">
+        <f t="shared" si="14"/>
+        <v>-2.440589104482187</v>
+      </c>
+      <c r="E482">
         <f t="shared" si="15"/>
-        <v>-2.440589104482187</v>
-      </c>
-      <c r="E482">
-        <f t="shared" si="14"/>
         <v>-3.251769321449149</v>
       </c>
     </row>
@@ -21018,11 +21031,11 @@
         <v>-3.0466966688753399</v>
       </c>
       <c r="D483">
+        <f t="shared" si="14"/>
+        <v>-2.4178241937268043</v>
+      </c>
+      <c r="E483">
         <f t="shared" si="15"/>
-        <v>-2.4178241937268043</v>
-      </c>
-      <c r="E483">
-        <f t="shared" si="14"/>
         <v>-3.2438887216146184</v>
       </c>
     </row>
@@ -21037,11 +21050,11 @@
         <v>-3.0432993541642301</v>
       </c>
       <c r="D484">
+        <f t="shared" si="14"/>
+        <v>-2.3947533101034311</v>
+      </c>
+      <c r="E484">
         <f t="shared" si="15"/>
-        <v>-2.3947533101034311</v>
-      </c>
-      <c r="E484">
-        <f t="shared" si="14"/>
         <v>-3.2358040281088312</v>
       </c>
     </row>
@@ -21056,11 +21069,11 @@
         <v>-3.03995534621833</v>
       </c>
       <c r="D485">
+        <f t="shared" si="14"/>
+        <v>-2.3713782105491799</v>
+      </c>
+      <c r="E485">
         <f t="shared" si="15"/>
-        <v>-2.3713782105491799</v>
-      </c>
-      <c r="E485">
-        <f t="shared" si="14"/>
         <v>-3.2275152409317869</v>
       </c>
     </row>
@@ -21075,11 +21088,11 @@
         <v>-3.0366711049391899</v>
       </c>
       <c r="D486">
+        <f t="shared" si="14"/>
+        <v>-2.3477006751683507</v>
+      </c>
+      <c r="E486">
         <f t="shared" si="15"/>
-        <v>-2.3477006751683507</v>
-      </c>
-      <c r="E486">
-        <f t="shared" si="14"/>
         <v>-3.2190223600834758</v>
       </c>
     </row>
@@ -21094,11 +21107,11 @@
         <v>-3.0334531391080102</v>
       </c>
       <c r="D487">
+        <f t="shared" si="14"/>
+        <v>-2.323722507096988</v>
+      </c>
+      <c r="E487">
         <f t="shared" si="15"/>
-        <v>-2.323722507096988</v>
-      </c>
-      <c r="E487">
-        <f t="shared" si="14"/>
         <v>-3.2103253855639169</v>
       </c>
     </row>
@@ -21113,11 +21126,11 @@
         <v>-3.0303080032007101</v>
       </c>
       <c r="D488">
+        <f t="shared" si="14"/>
+        <v>-2.2994455323654019</v>
+      </c>
+      <c r="E488">
         <f t="shared" si="15"/>
-        <v>-2.2994455323654019</v>
-      </c>
-      <c r="E488">
-        <f t="shared" si="14"/>
         <v>-3.2014243173731014</v>
       </c>
     </row>
@@ -21132,11 +21145,11 @@
         <v>-3.0272422940098802</v>
       </c>
       <c r="D489">
+        <f t="shared" si="14"/>
+        <v>-2.2748715997592082</v>
+      </c>
+      <c r="E489">
         <f t="shared" si="15"/>
-        <v>-2.2748715997592082</v>
-      </c>
-      <c r="E489">
-        <f t="shared" si="14"/>
         <v>-3.1923191555110284</v>
       </c>
     </row>
@@ -21151,11 +21164,11 @@
         <v>-3.0242626470700702</v>
       </c>
       <c r="D490">
+        <f t="shared" si="14"/>
+        <v>-2.2500025806785184</v>
+      </c>
+      <c r="E490">
         <f t="shared" si="15"/>
-        <v>-2.2500025806785184</v>
-      </c>
-      <c r="E490">
-        <f t="shared" si="14"/>
         <v>-3.1830098999776988</v>
       </c>
     </row>
@@ -21170,11 +21183,11 @@
         <v>-3.0213757328852799</v>
       </c>
       <c r="D491">
+        <f t="shared" si="14"/>
+        <v>-2.2248403689954213</v>
+      </c>
+      <c r="E491">
         <f t="shared" si="15"/>
-        <v>-2.2248403689954213</v>
-      </c>
-      <c r="E491">
-        <f t="shared" ref="E491:E542" si="16">IF(B491&gt;$J$7,$J$2*(B491+$J$5)^2+$J$4,$J$9*(B491+$J$12)^2+$J$11)</f>
         <v>-3.1734965507731121</v>
       </c>
     </row>
@@ -21189,11 +21202,11 @@
         <v>-3.0185882529561798</v>
       </c>
       <c r="D492">
+        <f t="shared" si="14"/>
+        <v>-2.1993868809097505</v>
+      </c>
+      <c r="E492">
         <f t="shared" si="15"/>
-        <v>-2.1993868809097505</v>
-      </c>
-      <c r="E492">
-        <f t="shared" si="16"/>
         <v>-3.1637791078972688</v>
       </c>
     </row>
@@ -21208,11 +21221,11 @@
         <v>-3.0159069356071</v>
       </c>
       <c r="D493">
+        <f t="shared" si="14"/>
+        <v>-2.1736440548031455</v>
+      </c>
+      <c r="E493">
         <f t="shared" si="15"/>
-        <v>-2.1736440548031455</v>
-      </c>
-      <c r="E493">
-        <f t="shared" si="16"/>
         <v>-3.1538575713501564</v>
       </c>
     </row>
@@ -21227,11 +21240,11 @@
         <v>-3.0133385316116401</v>
       </c>
       <c r="D494">
+        <f t="shared" si="14"/>
+        <v>-2.1476138510915388</v>
+      </c>
+      <c r="E494">
         <f t="shared" si="15"/>
-        <v>-2.1476138510915388</v>
-      </c>
-      <c r="E494">
-        <f t="shared" si="16"/>
         <v>-3.1437319411317985</v>
       </c>
     </row>
@@ -21246,11 +21259,11 @@
         <v>-3.0108898096180599</v>
       </c>
       <c r="D495">
+        <f t="shared" si="14"/>
+        <v>-2.1212982520756976</v>
+      </c>
+      <c r="E495">
         <f t="shared" si="15"/>
-        <v>-2.1212982520756976</v>
-      </c>
-      <c r="E495">
-        <f t="shared" si="16"/>
         <v>-3.1334022172421836</v>
       </c>
     </row>
@@ -21265,11 +21278,11 @@
         <v>-3.0085675513755699</v>
       </c>
       <c r="D496">
+        <f t="shared" si="14"/>
+        <v>-2.0946992617903661</v>
+      </c>
+      <c r="E496">
         <f t="shared" si="15"/>
-        <v>-2.0946992617903661</v>
-      </c>
-      <c r="E496">
-        <f t="shared" si="16"/>
         <v>-3.1228683996813116</v>
       </c>
     </row>
@@ -21284,11 +21297,11 @@
         <v>-3.0063785467631101</v>
       </c>
       <c r="D497">
+        <f t="shared" si="14"/>
+        <v>-2.0678189058516399</v>
+      </c>
+      <c r="E497">
         <f t="shared" si="15"/>
-        <v>-2.0678189058516399</v>
-      </c>
-      <c r="E497">
-        <f t="shared" si="16"/>
         <v>-3.1121304884491825</v>
       </c>
     </row>
@@ -21303,11 +21316,11 @@
         <v>-3.0043295886242198</v>
       </c>
       <c r="D498">
+        <f t="shared" si="14"/>
+        <v>-2.0406592313026946</v>
+      </c>
+      <c r="E498">
         <f t="shared" si="15"/>
-        <v>-2.0406592313026946</v>
-      </c>
-      <c r="E498">
-        <f t="shared" si="16"/>
         <v>-3.1011884835457963</v>
       </c>
     </row>
@@ -21322,11 +21335,11 @@
         <v>-3.0024274674114499</v>
       </c>
       <c r="D499">
+        <f t="shared" si="14"/>
+        <v>-2.0132223064578696</v>
+      </c>
+      <c r="E499">
         <f t="shared" si="15"/>
-        <v>-2.0132223064578696</v>
-      </c>
-      <c r="E499">
-        <f t="shared" si="16"/>
         <v>-3.0900423849711407</v>
       </c>
     </row>
@@ -21341,11 +21354,11 @@
         <v>-3.0006789656450699</v>
       </c>
       <c r="D500">
+        <f t="shared" si="14"/>
+        <v>-1.9855102207452791</v>
+      </c>
+      <c r="E500">
         <f t="shared" si="15"/>
-        <v>-1.9855102207452791</v>
-      </c>
-      <c r="E500">
-        <f t="shared" si="16"/>
         <v>-3.07869219272524</v>
       </c>
     </row>
@@ -21360,11 +21373,11 @@
         <v>-2.9990908521917401</v>
       </c>
       <c r="D501">
+        <f t="shared" si="14"/>
+        <v>-1.9575250845475152</v>
+      </c>
+      <c r="E501">
         <f t="shared" si="15"/>
-        <v>-1.9575250845475152</v>
-      </c>
-      <c r="E501">
-        <f t="shared" si="16"/>
         <v>-3.0671379068080826</v>
       </c>
     </row>
@@ -21379,11 +21392,11 @@
         <v>-2.9976698763703302</v>
       </c>
       <c r="D502">
+        <f t="shared" si="14"/>
+        <v>-1.9292690290410413</v>
+      </c>
+      <c r="E502">
         <f t="shared" si="15"/>
-        <v>-1.9292690290410413</v>
-      </c>
-      <c r="E502">
-        <f t="shared" si="16"/>
         <v>-3.0553795272196682</v>
       </c>
     </row>
@@ -21398,11 +21411,11 @@
         <v>-2.9964227618922399</v>
       </c>
       <c r="D503">
+        <f t="shared" si="14"/>
+        <v>-1.9007442060338855</v>
+      </c>
+      <c r="E503">
         <f t="shared" si="15"/>
-        <v>-1.9007442060338855</v>
-      </c>
-      <c r="E503">
-        <f t="shared" si="16"/>
         <v>-3.0434170539599976</v>
       </c>
     </row>
@@ -21417,11 +21430,11 @@
         <v>-2.9953562006447401</v>
       </c>
       <c r="D504">
+        <f t="shared" si="14"/>
+        <v>-1.871952787801761</v>
+      </c>
+      <c r="E504">
         <f t="shared" si="15"/>
-        <v>-1.871952787801761</v>
-      </c>
-      <c r="E504">
-        <f t="shared" si="16"/>
         <v>-3.0312504870290686</v>
       </c>
     </row>
@@ -21436,11 +21449,11 @@
         <v>-2.9944768463278701</v>
       </c>
       <c r="D505">
+        <f t="shared" si="14"/>
+        <v>-1.8428969669226305</v>
+      </c>
+      <c r="E505">
         <f t="shared" si="15"/>
-        <v>-1.8428969669226305</v>
-      </c>
-      <c r="E505">
-        <f t="shared" si="16"/>
         <v>-3.0188798264268835</v>
       </c>
     </row>
@@ -21455,11 +21468,11 @@
         <v>-2.9937913079556102</v>
       </c>
       <c r="D506">
+        <f t="shared" si="14"/>
+        <v>-1.813578956109716</v>
+      </c>
+      <c r="E506">
         <f t="shared" si="15"/>
-        <v>-1.813578956109716</v>
-      </c>
-      <c r="E506">
-        <f t="shared" si="16"/>
         <v>-3.0063050721534261</v>
       </c>
     </row>
@@ -21474,11 +21487,11 @@
         <v>-2.9933061432327102</v>
       </c>
       <c r="D507">
+        <f t="shared" si="14"/>
+        <v>-1.7840009880431236</v>
+      </c>
+      <c r="E507">
         <f t="shared" si="15"/>
-        <v>-1.7840009880431236</v>
-      </c>
-      <c r="E507">
-        <f t="shared" si="16"/>
         <v>-2.9935262242087268</v>
       </c>
     </row>
@@ -21493,11 +21506,11 @@
         <v>-2.99302785182108</v>
       </c>
       <c r="D508">
+        <f t="shared" si="14"/>
+        <v>-1.7541653151995971</v>
+      </c>
+      <c r="E508">
         <f t="shared" si="15"/>
-        <v>-1.7541653151995971</v>
-      </c>
-      <c r="E508">
-        <f t="shared" si="16"/>
         <v>-2.9805432825927696</v>
       </c>
     </row>
@@ -21512,11 +21525,11 @@
         <v>-2.99296286850916</v>
       </c>
       <c r="D509">
+        <f t="shared" si="14"/>
+        <v>-1.7240742096811381</v>
+      </c>
+      <c r="E509">
         <f t="shared" si="15"/>
-        <v>-1.7240742096811381</v>
-      </c>
-      <c r="E509">
-        <f t="shared" si="16"/>
         <v>-2.9673562473055566</v>
       </c>
     </row>
@@ -21531,11 +21544,11 @@
         <v>-2.9931175562995</v>
       </c>
       <c r="D510">
+        <f t="shared" si="14"/>
+        <v>-1.6937299630419393</v>
+      </c>
+      <c r="E510">
         <f t="shared" si="15"/>
-        <v>-1.6937299630419393</v>
-      </c>
-      <c r="E510">
-        <f t="shared" si="16"/>
         <v>-2.9539651183470852</v>
       </c>
     </row>
@@ -21550,11 +21563,11 @@
         <v>-2.9934981994307401</v>
       </c>
       <c r="D511">
+        <f t="shared" si="14"/>
+        <v>-1.6631348861138573</v>
+      </c>
+      <c r="E511">
         <f t="shared" si="15"/>
-        <v>-1.6631348861138573</v>
-      </c>
-      <c r="E511">
-        <f t="shared" si="16"/>
         <v>-2.9403698957173581</v>
       </c>
     </row>
@@ -21569,11 +21582,11 @@
         <v>-2.9941109963505999</v>
       </c>
       <c r="D512">
+        <f t="shared" si="14"/>
+        <v>-1.6322913088304229</v>
+      </c>
+      <c r="E512">
         <f t="shared" si="15"/>
-        <v>-1.6322913088304229</v>
-      </c>
-      <c r="E512">
-        <f t="shared" si="16"/>
         <v>-2.9265705794163575</v>
       </c>
     </row>
@@ -21588,11 +21601,11 @@
         <v>-2.9949620526579599</v>
       </c>
       <c r="D513">
+        <f t="shared" si="14"/>
+        <v>-1.6012015800495312</v>
+      </c>
+      <c r="E513">
         <f t="shared" si="15"/>
-        <v>-1.6012015800495312</v>
-      </c>
-      <c r="E513">
-        <f t="shared" si="16"/>
         <v>-2.9125671694441149</v>
       </c>
     </row>
@@ -21607,11 +21620,11 @@
         <v>-2.9960573740323202</v>
       </c>
       <c r="D514">
+        <f t="shared" si="14"/>
+        <v>-1.5698680673743657</v>
+      </c>
+      <c r="E514">
         <f t="shared" si="15"/>
-        <v>-1.5698680673743657</v>
-      </c>
-      <c r="E514">
-        <f t="shared" si="16"/>
         <v>-2.8983596658006165</v>
       </c>
     </row>
@@ -21626,11 +21639,11 @@
         <v>-2.9974028591704398</v>
       </c>
       <c r="D515">
-        <f t="shared" ref="D515:D542" si="17">IF(B515&gt;$J$7,$I$2*SIN($I$3*B515+$I$5)+$I$4,$I$9*SIN($I$10*B515+$I$12)+$I$11)</f>
+        <f t="shared" ref="D515:D542" si="16">IF(B515&gt;($J$7+$M$2),$I$2*SIN($I$3*B515+($I$5-$M$2))+$I$4,$I$9*SIN($I$10*B515+($I$12-$M$2))+$I$11)</f>
         <v>-1.5382931569732206</v>
       </c>
       <c r="E515">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="E515:E542" si="17">IF(B515&gt;($J$7+$M$2),$J$2*(B515+($J$5-$M$2))^2+$J$4,$J$9*(B515+($J$12-$M$2))^2+$J$11)</f>
         <v>-2.8839480684858598</v>
       </c>
     </row>
@@ -21645,11 +21658,11 @@
         <v>-2.99900429274925</v>
       </c>
       <c r="D516">
+        <f t="shared" si="16"/>
+        <v>-1.506479253397782</v>
+      </c>
+      <c r="E516">
         <f t="shared" si="17"/>
-        <v>-1.506479253397782</v>
-      </c>
-      <c r="E516">
-        <f t="shared" si="16"/>
         <v>-2.8693323774998474</v>
       </c>
     </row>
@@ -21664,11 +21677,11 @@
         <v>-3.0008673384367399</v>
       </c>
       <c r="D517">
+        <f t="shared" si="16"/>
+        <v>-1.4744287793999704</v>
+      </c>
+      <c r="E517">
         <f t="shared" si="17"/>
-        <v>-1.4744287793999704</v>
-      </c>
-      <c r="E517">
-        <f t="shared" si="16"/>
         <v>-2.8545125928425765</v>
       </c>
     </row>
@@ -21683,11 +21696,11 @@
         <v>-3.0029975319703501</v>
       </c>
       <c r="D518">
+        <f t="shared" si="16"/>
+        <v>-1.4421441757474733</v>
+      </c>
+      <c r="E518">
         <f t="shared" si="17"/>
-        <v>-1.4421441757474733</v>
-      </c>
-      <c r="E518">
-        <f t="shared" si="16"/>
         <v>-2.8394887145140499</v>
       </c>
     </row>
@@ -21702,11 +21715,11 @@
         <v>-3.0054002743252699</v>
       </c>
       <c r="D519">
+        <f t="shared" si="16"/>
+        <v>-1.4096279010378159</v>
+      </c>
+      <c r="E519">
         <f t="shared" si="17"/>
-        <v>-1.4096279010378159</v>
-      </c>
-      <c r="E519">
-        <f t="shared" si="16"/>
         <v>-2.8242607425142485</v>
       </c>
     </row>
@@ -21721,11 +21734,11 @@
         <v>-3.0080808249938502</v>
       </c>
       <c r="D520">
+        <f t="shared" si="16"/>
+        <v>-1.3768824315112864</v>
+      </c>
+      <c r="E520">
         <f t="shared" si="17"/>
-        <v>-1.3768824315112864</v>
-      </c>
-      <c r="E520">
-        <f t="shared" si="16"/>
         <v>-2.8088286768432065</v>
       </c>
     </row>
@@ -21740,11 +21753,11 @@
         <v>-3.0110442953965899</v>
       </c>
       <c r="D521">
+        <f t="shared" si="16"/>
+        <v>-1.343910260862125</v>
+      </c>
+      <c r="E521">
         <f t="shared" si="17"/>
-        <v>-1.343910260862125</v>
-      </c>
-      <c r="E521">
-        <f t="shared" si="16"/>
         <v>-2.7931925175009087</v>
       </c>
     </row>
@@ -21759,11 +21772,11 @@
         <v>-3.01429564244861</v>
       </c>
       <c r="D522">
+        <f t="shared" si="16"/>
+        <v>-1.3107139000487864</v>
+      </c>
+      <c r="E522">
         <f t="shared" si="17"/>
-        <v>-1.3107139000487864</v>
-      </c>
-      <c r="E522">
-        <f t="shared" si="16"/>
         <v>-2.777352264487353</v>
       </c>
     </row>
@@ -21778,11 +21791,11 @@
         <v>-3.0178396623005099</v>
       </c>
       <c r="D523">
+        <f t="shared" si="16"/>
+        <v>-1.2772958771026763</v>
+      </c>
+      <c r="E523">
         <f t="shared" si="17"/>
-        <v>-1.2772958771026763</v>
-      </c>
-      <c r="E523">
-        <f t="shared" si="16"/>
         <v>-2.761307917802541</v>
       </c>
     </row>
@@ -21797,11 +21810,11 @@
         <v>-3.0216809842755499</v>
       </c>
       <c r="D524">
+        <f t="shared" si="16"/>
+        <v>-1.2436587369356138</v>
+      </c>
+      <c r="E524">
         <f t="shared" si="17"/>
-        <v>-1.2436587369356138</v>
-      </c>
-      <c r="E524">
-        <f t="shared" si="16"/>
         <v>-2.7450594774464712</v>
       </c>
     </row>
@@ -21816,11 +21829,11 @@
         <v>-3.0258240650250001</v>
       </c>
       <c r="D525">
+        <f t="shared" si="16"/>
+        <v>-1.2098050411460268</v>
+      </c>
+      <c r="E525">
         <f t="shared" si="17"/>
-        <v>-1.2098050411460268</v>
-      </c>
-      <c r="E525">
-        <f t="shared" si="16"/>
         <v>-2.7286069434191256</v>
       </c>
     </row>
@@ -21835,11 +21848,11 @@
         <v>-3.0302731829198399</v>
       </c>
       <c r="D526">
+        <f t="shared" si="16"/>
+        <v>-1.1757373678239951</v>
+      </c>
+      <c r="E526">
         <f t="shared" si="17"/>
-        <v>-1.1757373678239951</v>
-      </c>
-      <c r="E526">
-        <f t="shared" si="16"/>
         <v>-2.7119503157205425</v>
       </c>
     </row>
@@ -21854,11 +21867,11 @@
         <v>-3.03503243269948</v>
       </c>
       <c r="D527">
+        <f t="shared" si="16"/>
+        <v>-1.1414583113546959</v>
+      </c>
+      <c r="E527">
         <f t="shared" si="17"/>
-        <v>-1.1414583113546959</v>
-      </c>
-      <c r="E527">
-        <f t="shared" si="16"/>
         <v>-2.6950895943507014</v>
       </c>
     </row>
@@ -21873,11 +21886,11 @@
         <v>-3.0401057203958399</v>
       </c>
       <c r="D528">
+        <f t="shared" si="16"/>
+        <v>-1.106970482221</v>
+      </c>
+      <c r="E528">
         <f t="shared" si="17"/>
-        <v>-1.106970482221</v>
-      </c>
-      <c r="E528">
-        <f t="shared" si="16"/>
         <v>-2.6780247793096041</v>
       </c>
     </row>
@@ -21892,11 +21905,11 @@
         <v>-3.0454967585452799</v>
       </c>
       <c r="D529">
+        <f t="shared" si="16"/>
+        <v>-1.0722765068046245</v>
+      </c>
+      <c r="E529">
         <f t="shared" si="17"/>
-        <v>-1.0722765068046245</v>
-      </c>
-      <c r="E529">
-        <f t="shared" si="16"/>
         <v>-2.6607558705972485</v>
       </c>
     </row>
@@ -21911,11 +21924,11 @@
         <v>-3.0512090617250802</v>
       </c>
       <c r="D530">
+        <f t="shared" si="16"/>
+        <v>-1.037379027186113</v>
+      </c>
+      <c r="E530">
         <f t="shared" si="17"/>
-        <v>-1.037379027186113</v>
-      </c>
-      <c r="E530">
-        <f t="shared" si="16"/>
         <v>-2.6432828682136376</v>
       </c>
     </row>
@@ -21930,11 +21943,11 @@
         <v>-3.05724594238806</v>
       </c>
       <c r="D531">
+        <f t="shared" si="16"/>
+        <v>-1.0022807009436137</v>
+      </c>
+      <c r="E531">
         <f t="shared" si="17"/>
-        <v>-1.0022807009436137</v>
-      </c>
-      <c r="E531">
-        <f t="shared" si="16"/>
         <v>-2.6256057721587482</v>
       </c>
     </row>
@@ -21949,11 +21962,11 @@
         <v>-3.0636105070582502</v>
       </c>
       <c r="D532">
+        <f t="shared" si="16"/>
+        <v>-0.96698420095063709</v>
+      </c>
+      <c r="E532">
         <f t="shared" si="17"/>
-        <v>-0.96698420095063709</v>
-      </c>
-      <c r="E532">
-        <f t="shared" si="16"/>
         <v>-2.6077245824326218</v>
       </c>
     </row>
@@ -21968,11 +21981,11 @@
         <v>-3.0703056528780199</v>
       </c>
       <c r="D533">
+        <f t="shared" si="16"/>
+        <v>-0.93149221517227909</v>
+      </c>
+      <c r="E533">
         <f t="shared" si="17"/>
-        <v>-0.93149221517227909</v>
-      </c>
-      <c r="E533">
-        <f t="shared" si="16"/>
         <v>-2.5896392990352393</v>
       </c>
     </row>
@@ -21987,11 +22000,11 @@
         <v>-3.07733406449253</v>
       </c>
       <c r="D534">
+        <f t="shared" si="16"/>
+        <v>-0.89580744646065735</v>
+      </c>
+      <c r="E534">
         <f t="shared" si="17"/>
-        <v>-0.89580744646065735</v>
-      </c>
-      <c r="E534">
-        <f t="shared" si="16"/>
         <v>-2.5713499219665987</v>
       </c>
     </row>
@@ -22006,11 +22019,11 @@
         <v>-3.0846982113332202</v>
       </c>
       <c r="D535">
+        <f t="shared" si="16"/>
+        <v>-0.85993261234908358</v>
+      </c>
+      <c r="E535">
         <f t="shared" si="17"/>
-        <v>-0.85993261234908358</v>
-      </c>
-      <c r="E535">
-        <f t="shared" si="16"/>
         <v>-2.552856451226702</v>
       </c>
     </row>
@@ -22025,11 +22038,11 @@
         <v>-3.0924003452656801</v>
       </c>
       <c r="D536">
+        <f t="shared" si="16"/>
+        <v>-0.82387044484505934</v>
+      </c>
+      <c r="E536">
         <f t="shared" si="17"/>
-        <v>-0.82387044484505934</v>
-      </c>
-      <c r="E536">
-        <f t="shared" si="16"/>
         <v>-2.5341588868155478</v>
       </c>
     </row>
@@ -22044,11 +22057,11 @@
         <v>-3.1004424986268999</v>
       </c>
       <c r="D537">
+        <f t="shared" si="16"/>
+        <v>-0.78762369022226464</v>
+      </c>
+      <c r="E537">
         <f t="shared" si="17"/>
-        <v>-0.78762369022226464</v>
-      </c>
-      <c r="E537">
-        <f t="shared" si="16"/>
         <v>-2.515257228733137</v>
       </c>
     </row>
@@ -22063,11 +22076,11 @@
         <v>-3.1088264826523799</v>
       </c>
       <c r="D538">
+        <f t="shared" si="16"/>
+        <v>-0.75119510881135731</v>
+      </c>
+      <c r="E538">
         <f t="shared" si="17"/>
-        <v>-0.75119510881135731</v>
-      </c>
-      <c r="E538">
-        <f t="shared" si="16"/>
         <v>-2.4961514769794455</v>
       </c>
     </row>
@@ -22082,11 +22095,11 @@
         <v>-3.1175538862945702</v>
       </c>
       <c r="D539">
+        <f t="shared" si="16"/>
+        <v>-0.714587474789937</v>
+      </c>
+      <c r="E539">
         <f t="shared" si="17"/>
-        <v>-0.714587474789937</v>
-      </c>
-      <c r="E539">
-        <f t="shared" si="16"/>
         <v>-2.476841631554521</v>
       </c>
     </row>
@@ -22101,11 +22114,11 @@
         <v>-3.1266260754375699</v>
       </c>
       <c r="D540">
+        <f t="shared" si="16"/>
+        <v>-0.67780357597101393</v>
+      </c>
+      <c r="E540">
         <f t="shared" si="17"/>
-        <v>-0.67780357597101393</v>
-      </c>
-      <c r="E540">
-        <f t="shared" si="16"/>
         <v>-2.457327692458338</v>
       </c>
     </row>
@@ -22120,11 +22133,11 @@
         <v>-3.1360441925000302</v>
       </c>
       <c r="D541">
+        <f t="shared" si="16"/>
+        <v>-0.64084621359091321</v>
+      </c>
+      <c r="E541">
         <f t="shared" si="17"/>
-        <v>-0.64084621359091321</v>
-      </c>
-      <c r="E541">
-        <f t="shared" si="16"/>
         <v>-2.4376096596908989</v>
       </c>
     </row>
@@ -22139,11 +22152,11 @@
         <v>-3.1458091564326098</v>
       </c>
       <c r="D542">
+        <f t="shared" si="16"/>
+        <v>-0.60371820209585447</v>
+      </c>
+      <c r="E542">
         <f t="shared" si="17"/>
-        <v>-0.60371820209585447</v>
-      </c>
-      <c r="E542">
-        <f t="shared" si="16"/>
         <v>-2.4176875332522023</v>
       </c>
     </row>

</xml_diff>